<commit_message>
Update Effort Estimate documents
</commit_message>
<xml_diff>
--- a/documentation/CS451R.Group14.EffortEstimate.xlsx
+++ b/documentation/CS451R.Group14.EffortEstimate.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="110">
   <si>
     <t>Note: Beyond Iteration 2, nothing is changed.</t>
   </si>
@@ -269,6 +269,9 @@
     </r>
   </si>
   <si>
+    <t>Done</t>
+  </si>
+  <si>
     <t>Set up double proxy for HTTP server</t>
   </si>
   <si>
@@ -283,9 +286,6 @@
     <t>Zach Zoltek</t>
   </si>
   <si>
-    <t>Done</t>
-  </si>
-  <si>
     <t>Implement foundational HTTP logic</t>
   </si>
   <si>
@@ -298,7 +298,7 @@
     <t>Write user token handling locally</t>
   </si>
   <si>
-    <t>Yazdan Riazai</t>
+    <t>Yazdan Riazi</t>
   </si>
   <si>
     <t>Todo</t>
@@ -323,9 +323,6 @@
   </si>
   <si>
     <t>System and Environment Testing</t>
-  </si>
-  <si>
-    <t>IR</t>
   </si>
   <si>
     <t>Bug fixes as required</t>
@@ -360,19 +357,37 @@
     <t>Implement any design changes</t>
   </si>
   <si>
-    <t>Risk analysis</t>
+    <t>IR</t>
   </si>
   <si>
     <t>-</t>
   </si>
   <si>
+    <t>Risk analysis</t>
+  </si>
+  <si>
     <t>Design container format (schedule)</t>
   </si>
   <si>
-    <t>Alivia Dutcher, Samuel Lim</t>
+    <r>
+      <t xml:space="preserve">Alivia Dutcher, </t>
+    </r>
+    <r>
+      <rPr/>
+      <t>Samuel Lim</t>
+    </r>
   </si>
   <si>
     <t>Design drop-in format parsing</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Alivia Dutcher, </t>
+    </r>
+    <r>
+      <rPr/>
+      <t>Samuel Lim</t>
+    </r>
   </si>
   <si>
     <t>Create UI design for main page</t>
@@ -381,7 +396,13 @@
     <t>Review requirements</t>
   </si>
   <si>
-    <t>Alivia Dutcher, Zach Zoltek, Samuel Lim</t>
+    <r>
+      <t xml:space="preserve">Alivia Dutcher, </t>
+    </r>
+    <r>
+      <rPr/>
+      <t>Zach Zoltek, Samuel Lim</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Connect client and session HTTP logic
@@ -402,9 +423,6 @@
   </si>
   <si>
     <t>Handle basic token generation</t>
-  </si>
-  <si>
-    <t>Yazdan Riazi</t>
   </si>
   <si>
     <t>Implement design structure for main page</t>
@@ -436,25 +454,74 @@
     <t>Iteration 3:</t>
   </si>
   <si>
-    <t>Create UI design for vendor locations</t>
+    <r>
+      <t xml:space="preserve">Samuel Lim, </t>
+    </r>
+    <r>
+      <rPr/>
+      <t>Alivia Dutcher</t>
+    </r>
   </si>
   <si>
-    <t>Design data structure for RSS location list</t>
+    <t>*Snowplow from Iteration #2</t>
   </si>
   <si>
-    <t>Develop code for processing vendor locations</t>
+    <t>Design data structure for schedule constraints</t>
   </si>
   <si>
-    <t>Implement vendor map display</t>
+    <t>Develop code for processing scheduling data</t>
   </si>
   <si>
-    <t>Display vendor information</t>
+    <r>
+      <t>Alivia Dutcher,</t>
+    </r>
+    <r>
+      <rPr/>
+      <t xml:space="preserve"> Samuel Lim</t>
+    </r>
+  </si>
+  <si>
+    <t>Implement client-API integration</t>
+  </si>
+  <si>
+    <t>Display scheduling information</t>
   </si>
   <si>
     <t>Acceptance Testing</t>
   </si>
   <si>
     <t>Tester, Project Manager</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t>Zach Zoltek</t>
+    </r>
+    <r>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <t>Samuel Lim</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t>Alivia Dutcher</t>
+    </r>
+    <r>
+      <t>, Zach Zoltek</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -707,7 +774,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="167">
+  <cellXfs count="170">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -852,11 +919,11 @@
     <xf borderId="7" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="10" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="10" fillId="3" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="10" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -954,6 +1021,9 @@
     <xf borderId="12" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="11" fillId="5" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
@@ -962,12 +1032,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="11" fillId="5" fontId="9" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="11" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -1001,9 +1065,6 @@
     </xf>
     <xf borderId="5" fillId="5" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="5" fontId="9" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="5" fillId="5" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
@@ -1050,7 +1111,7 @@
     <xf borderId="12" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="10" fillId="3" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="10" fillId="3" fontId="9" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="10" fillId="3" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -1071,20 +1132,17 @@
     <xf borderId="6" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="4" fillId="3" fontId="9" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="4" fillId="3" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="4" fillId="3" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf borderId="11" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="11" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="11" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="11" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="11" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -1098,10 +1156,10 @@
     <xf borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="2" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="3" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1110,7 +1168,7 @@
     <xf borderId="3" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="5" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="5" fontId="9" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="5" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -1119,25 +1177,31 @@
     <xf borderId="11" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="11" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="11" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="10" fillId="5" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="11" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="10" fillId="5" fontId="9" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="5" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="11" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="11" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="5" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -1148,6 +1212,12 @@
     </xf>
     <xf borderId="4" fillId="5" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="11" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -1173,17 +1243,23 @@
     <xf borderId="1" fillId="4" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="2" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="1" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="5" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="1" fillId="5" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="14" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="5" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="9" fillId="6" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
@@ -1442,7 +1518,9 @@
     <col customWidth="1" min="7" max="7" width="11.57"/>
     <col customWidth="1" min="8" max="8" width="11.71"/>
     <col customWidth="1" min="9" max="9" width="10.71"/>
-    <col customWidth="1" min="10" max="32" width="9.0"/>
+    <col customWidth="1" min="10" max="17" width="9.0"/>
+    <col customWidth="1" min="18" max="18" width="38.0"/>
+    <col customWidth="1" min="19" max="32" width="9.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1851,7 +1929,7 @@
       <c r="O9" s="46">
         <v>0.5</v>
       </c>
-      <c r="P9" s="48">
+      <c r="P9" s="46">
         <v>0.2</v>
       </c>
       <c r="Q9" s="45">
@@ -1986,7 +2064,7 @@
       <c r="H12" s="36"/>
       <c r="I12" s="38">
         <f>SUM(H13:H19)</f>
-        <v>11</v>
+        <v>16.5</v>
       </c>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
@@ -2083,7 +2161,7 @@
       <c r="E14" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="49">
+      <c r="F14" s="48">
         <v>2.0</v>
       </c>
       <c r="G14" s="44"/>
@@ -2191,25 +2269,33 @@
       <c r="E16" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="49">
+      <c r="F16" s="48">
         <v>5.0</v>
       </c>
       <c r="G16" s="44"/>
       <c r="H16" s="45">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="I16" s="44"/>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
-      <c r="M16" s="46"/>
-      <c r="N16" s="46"/>
-      <c r="O16" s="45"/>
-      <c r="P16" s="46"/>
+      <c r="M16" s="49">
+        <v>1.5</v>
+      </c>
+      <c r="N16" s="49">
+        <v>1.5</v>
+      </c>
+      <c r="O16" s="49">
+        <v>1.5</v>
+      </c>
+      <c r="P16" s="49">
+        <v>1.0</v>
+      </c>
       <c r="Q16" s="45">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
@@ -2239,7 +2325,7 @@
       <c r="E17" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="49">
+      <c r="F17" s="48">
         <v>4.0</v>
       </c>
       <c r="G17" s="44"/>
@@ -2481,24 +2567,24 @@
         <v>1.7</v>
       </c>
       <c r="I22" s="81"/>
-      <c r="J22" s="17" t="s">
+      <c r="J22" s="82" t="s">
         <v>54</v>
       </c>
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
-      <c r="M22" s="82">
+      <c r="M22" s="83">
         <v>0.6</v>
       </c>
-      <c r="N22" s="82">
+      <c r="N22" s="83">
         <v>0.4</v>
       </c>
-      <c r="O22" s="82">
+      <c r="O22" s="83">
         <v>0.5</v>
       </c>
-      <c r="P22" s="82">
+      <c r="P22" s="83">
         <v>0.2</v>
       </c>
-      <c r="Q22" s="83">
+      <c r="Q22" s="84">
         <f t="shared" si="1"/>
         <v>1.7</v>
       </c>
@@ -2518,7 +2604,7 @@
       <c r="AE22" s="6"/>
       <c r="AF22" s="6"/>
     </row>
-    <row r="23" ht="29.25" customHeight="1">
+    <row r="23" ht="33.75" customHeight="1">
       <c r="A23" s="68"/>
       <c r="B23" s="74"/>
       <c r="C23" s="75" t="s">
@@ -2539,24 +2625,24 @@
         <v>13</v>
       </c>
       <c r="I23" s="79"/>
-      <c r="J23" s="84" t="s">
-        <v>54</v>
+      <c r="J23" s="82" t="s">
+        <v>57</v>
       </c>
       <c r="K23" s="85"/>
       <c r="L23" s="5"/>
-      <c r="M23" s="82">
+      <c r="M23" s="83">
         <v>4.0</v>
       </c>
-      <c r="N23" s="86">
+      <c r="N23" s="83">
         <v>3.0</v>
       </c>
-      <c r="O23" s="82">
+      <c r="O23" s="83">
         <v>3.5</v>
       </c>
-      <c r="P23" s="82">
+      <c r="P23" s="83">
         <v>2.5</v>
       </c>
-      <c r="Q23" s="83">
+      <c r="Q23" s="84">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
@@ -2579,14 +2665,14 @@
     <row r="24" ht="15.0" customHeight="1">
       <c r="A24" s="68"/>
       <c r="B24" s="74"/>
-      <c r="C24" s="87" t="s">
-        <v>57</v>
+      <c r="C24" s="86" t="s">
+        <v>58</v>
       </c>
       <c r="D24" s="76" t="s">
         <v>52</v>
       </c>
       <c r="E24" s="77" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F24" s="78">
         <v>2.0</v>
@@ -2597,20 +2683,20 @@
         <v>0.8</v>
       </c>
       <c r="I24" s="79"/>
-      <c r="J24" s="84" t="s">
-        <v>54</v>
+      <c r="J24" s="82" t="s">
+        <v>57</v>
       </c>
       <c r="K24" s="85"/>
       <c r="L24" s="5"/>
-      <c r="M24" s="82">
+      <c r="M24" s="83">
         <v>0.5</v>
       </c>
-      <c r="N24" s="83"/>
-      <c r="O24" s="86">
+      <c r="N24" s="84"/>
+      <c r="O24" s="83">
         <v>0.3</v>
       </c>
-      <c r="P24" s="83"/>
-      <c r="Q24" s="83">
+      <c r="P24" s="84"/>
+      <c r="Q24" s="84">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
@@ -2633,14 +2719,14 @@
     <row r="25" ht="15.0" customHeight="1">
       <c r="A25" s="68"/>
       <c r="B25" s="74"/>
-      <c r="C25" s="88" t="s">
-        <v>59</v>
+      <c r="C25" s="87" t="s">
+        <v>60</v>
       </c>
       <c r="D25" s="76" t="s">
         <v>52</v>
       </c>
       <c r="E25" s="77" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F25" s="78">
         <v>1.0</v>
@@ -2651,24 +2737,24 @@
         <v>0.6</v>
       </c>
       <c r="I25" s="79"/>
-      <c r="J25" s="84" t="s">
-        <v>61</v>
+      <c r="J25" s="85" t="s">
+        <v>57</v>
       </c>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
-      <c r="M25" s="82">
+      <c r="M25" s="83">
         <v>0.3</v>
       </c>
-      <c r="N25" s="86">
+      <c r="N25" s="83">
         <v>0.0</v>
       </c>
-      <c r="O25" s="82">
+      <c r="O25" s="83">
         <v>0.3</v>
       </c>
-      <c r="P25" s="86">
+      <c r="P25" s="83">
         <v>0.0</v>
       </c>
-      <c r="Q25" s="83">
+      <c r="Q25" s="84">
         <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
@@ -2690,15 +2776,15 @@
     </row>
     <row r="26" ht="15.0" customHeight="1">
       <c r="A26" s="68"/>
-      <c r="B26" s="89"/>
-      <c r="C26" s="88" t="s">
+      <c r="B26" s="88"/>
+      <c r="C26" s="87" t="s">
         <v>62</v>
       </c>
       <c r="D26" s="76" t="s">
         <v>52</v>
       </c>
       <c r="E26" s="77" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F26" s="78">
         <v>12.0</v>
@@ -2709,18 +2795,18 @@
         <v>0.3</v>
       </c>
       <c r="I26" s="79"/>
-      <c r="J26" s="84" t="s">
+      <c r="J26" s="85" t="s">
         <v>54</v>
       </c>
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
-      <c r="M26" s="86">
+      <c r="M26" s="83">
         <v>0.3</v>
       </c>
-      <c r="N26" s="83"/>
-      <c r="O26" s="83"/>
-      <c r="P26" s="82"/>
-      <c r="Q26" s="83">
+      <c r="N26" s="84"/>
+      <c r="O26" s="84"/>
+      <c r="P26" s="83"/>
+      <c r="Q26" s="84">
         <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
@@ -2742,8 +2828,8 @@
     </row>
     <row r="27" ht="15.0" customHeight="1">
       <c r="A27" s="68"/>
-      <c r="B27" s="89"/>
-      <c r="C27" s="87" t="s">
+      <c r="B27" s="88"/>
+      <c r="C27" s="86" t="s">
         <v>63</v>
       </c>
       <c r="D27" s="76" t="s">
@@ -2761,18 +2847,18 @@
         <v>0.3</v>
       </c>
       <c r="I27" s="79"/>
-      <c r="J27" s="84" t="s">
+      <c r="J27" s="85" t="s">
         <v>54</v>
       </c>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
-      <c r="M27" s="86">
+      <c r="M27" s="83">
         <v>0.3</v>
       </c>
-      <c r="N27" s="83"/>
-      <c r="O27" s="83"/>
-      <c r="P27" s="82"/>
-      <c r="Q27" s="83">
+      <c r="N27" s="84"/>
+      <c r="O27" s="84"/>
+      <c r="P27" s="83"/>
+      <c r="Q27" s="84">
         <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
@@ -2794,8 +2880,8 @@
     </row>
     <row r="28" ht="15.0" customHeight="1">
       <c r="A28" s="68"/>
-      <c r="B28" s="89"/>
-      <c r="C28" s="87" t="s">
+      <c r="B28" s="88"/>
+      <c r="C28" s="86" t="s">
         <v>65</v>
       </c>
       <c r="D28" s="76" t="s">
@@ -2813,16 +2899,16 @@
         <v>0</v>
       </c>
       <c r="I28" s="79"/>
-      <c r="J28" s="84" t="s">
+      <c r="J28" s="85" t="s">
         <v>67</v>
       </c>
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
-      <c r="M28" s="83"/>
-      <c r="N28" s="83"/>
-      <c r="O28" s="83"/>
-      <c r="P28" s="82"/>
-      <c r="Q28" s="83">
+      <c r="M28" s="84"/>
+      <c r="N28" s="84"/>
+      <c r="O28" s="84"/>
+      <c r="P28" s="83"/>
+      <c r="Q28" s="84">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2844,7 +2930,7 @@
     </row>
     <row r="29" ht="15.0" customHeight="1">
       <c r="A29" s="68"/>
-      <c r="B29" s="89"/>
+      <c r="B29" s="88"/>
       <c r="C29" s="75" t="s">
         <v>68</v>
       </c>
@@ -2852,7 +2938,7 @@
         <v>52</v>
       </c>
       <c r="E29" s="77" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F29" s="78">
         <v>6.0</v>
@@ -2863,16 +2949,16 @@
         <v>0</v>
       </c>
       <c r="I29" s="79"/>
-      <c r="J29" s="84" t="s">
+      <c r="J29" s="85" t="s">
         <v>67</v>
       </c>
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
-      <c r="M29" s="83"/>
-      <c r="N29" s="83"/>
-      <c r="O29" s="83"/>
-      <c r="P29" s="82"/>
-      <c r="Q29" s="83">
+      <c r="M29" s="84"/>
+      <c r="N29" s="84"/>
+      <c r="O29" s="84"/>
+      <c r="P29" s="83"/>
+      <c r="Q29" s="84">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2894,37 +2980,37 @@
     </row>
     <row r="30" ht="15.0" customHeight="1">
       <c r="A30" s="68"/>
-      <c r="B30" s="90"/>
-      <c r="C30" s="91" t="s">
+      <c r="B30" s="89"/>
+      <c r="C30" s="90" t="s">
         <v>69</v>
       </c>
-      <c r="D30" s="92" t="s">
+      <c r="D30" s="91" t="s">
         <v>52</v>
       </c>
-      <c r="E30" s="93" t="s">
+      <c r="E30" s="92" t="s">
         <v>70</v>
       </c>
-      <c r="F30" s="94">
+      <c r="F30" s="93">
         <v>4.0</v>
       </c>
-      <c r="G30" s="95"/>
-      <c r="H30" s="96">
+      <c r="G30" s="94"/>
+      <c r="H30" s="95">
         <f t="shared" si="4"/>
         <v>0.3</v>
       </c>
-      <c r="I30" s="95"/>
-      <c r="J30" s="84" t="s">
+      <c r="I30" s="94"/>
+      <c r="J30" s="85" t="s">
         <v>54</v>
       </c>
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
-      <c r="M30" s="97"/>
-      <c r="N30" s="97"/>
-      <c r="O30" s="98">
+      <c r="M30" s="96"/>
+      <c r="N30" s="96"/>
+      <c r="O30" s="97">
         <v>0.3</v>
       </c>
-      <c r="P30" s="99"/>
-      <c r="Q30" s="97">
+      <c r="P30" s="97"/>
+      <c r="Q30" s="96">
         <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
@@ -2946,18 +3032,18 @@
     </row>
     <row r="31" ht="15.0" customHeight="1">
       <c r="A31" s="68"/>
-      <c r="B31" s="100" t="s">
+      <c r="B31" s="98" t="s">
         <v>71</v>
       </c>
-      <c r="C31" s="101"/>
+      <c r="C31" s="99"/>
       <c r="D31" s="70"/>
       <c r="E31" s="70"/>
-      <c r="F31" s="102"/>
+      <c r="F31" s="100"/>
       <c r="G31" s="37">
         <f>SUM(F32:F34)</f>
         <v>10</v>
       </c>
-      <c r="H31" s="102"/>
+      <c r="H31" s="100"/>
       <c r="I31" s="38">
         <f>SUM(H32:H34)</f>
         <v>5.2</v>
@@ -2991,17 +3077,17 @@
     </row>
     <row r="32" ht="15.0" customHeight="1">
       <c r="A32" s="68"/>
-      <c r="B32" s="89"/>
-      <c r="C32" s="87" t="s">
+      <c r="B32" s="88"/>
+      <c r="C32" s="86" t="s">
         <v>72</v>
       </c>
       <c r="D32" s="76" t="s">
         <v>43</v>
       </c>
       <c r="E32" s="77" t="s">
-        <v>60</v>
-      </c>
-      <c r="F32" s="103">
+        <v>61</v>
+      </c>
+      <c r="F32" s="101">
         <v>2.0</v>
       </c>
       <c r="G32" s="79"/>
@@ -3010,24 +3096,24 @@
         <v>1.7</v>
       </c>
       <c r="I32" s="79"/>
-      <c r="J32" s="84" t="s">
-        <v>73</v>
+      <c r="J32" s="82" t="s">
+        <v>57</v>
       </c>
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
-      <c r="M32" s="104">
+      <c r="M32" s="102">
         <v>0.5</v>
       </c>
-      <c r="N32" s="104">
+      <c r="N32" s="102">
         <v>0.5</v>
       </c>
-      <c r="O32" s="104">
+      <c r="O32" s="102">
         <v>0.5</v>
       </c>
-      <c r="P32" s="104">
+      <c r="P32" s="102">
         <v>0.2</v>
       </c>
-      <c r="Q32" s="105">
+      <c r="Q32" s="103">
         <f t="shared" si="1"/>
         <v>1.7</v>
       </c>
@@ -3049,15 +3135,15 @@
     </row>
     <row r="33" ht="15.0" customHeight="1">
       <c r="A33" s="68"/>
-      <c r="B33" s="89"/>
-      <c r="C33" s="87" t="s">
+      <c r="B33" s="88"/>
+      <c r="C33" s="86" t="s">
+        <v>73</v>
+      </c>
+      <c r="D33" s="76" t="s">
         <v>74</v>
       </c>
-      <c r="D33" s="76" t="s">
+      <c r="E33" s="104" t="s">
         <v>75</v>
-      </c>
-      <c r="E33" s="106" t="s">
-        <v>76</v>
       </c>
       <c r="F33" s="78">
         <v>3.0</v>
@@ -3068,24 +3154,24 @@
         <v>0</v>
       </c>
       <c r="I33" s="79"/>
-      <c r="J33" s="84" t="s">
-        <v>77</v>
+      <c r="J33" s="85" t="s">
+        <v>76</v>
       </c>
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
-      <c r="M33" s="104">
+      <c r="M33" s="102">
         <v>0.0</v>
       </c>
-      <c r="N33" s="104">
+      <c r="N33" s="102">
         <v>0.0</v>
       </c>
-      <c r="O33" s="104">
+      <c r="O33" s="102">
         <v>0.0</v>
       </c>
-      <c r="P33" s="104">
+      <c r="P33" s="102">
         <v>0.0</v>
       </c>
-      <c r="Q33" s="105">
+      <c r="Q33" s="103">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3107,9 +3193,9 @@
     </row>
     <row r="34" ht="15.0" customHeight="1">
       <c r="A34" s="68"/>
-      <c r="B34" s="89"/>
+      <c r="B34" s="88"/>
       <c r="C34" s="75" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D34" s="76" t="s">
         <v>20</v>
@@ -3126,24 +3212,24 @@
         <v>3.5</v>
       </c>
       <c r="I34" s="79"/>
-      <c r="J34" s="84" t="s">
-        <v>61</v>
+      <c r="J34" s="85" t="s">
+        <v>57</v>
       </c>
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
-      <c r="M34" s="104">
+      <c r="M34" s="102">
         <v>2.0</v>
       </c>
-      <c r="N34" s="104">
+      <c r="N34" s="102">
         <v>0.5</v>
       </c>
-      <c r="O34" s="104">
+      <c r="O34" s="102">
         <v>0.5</v>
       </c>
-      <c r="P34" s="104">
+      <c r="P34" s="102">
         <v>0.5</v>
       </c>
-      <c r="Q34" s="105">
+      <c r="Q34" s="103">
         <f t="shared" si="1"/>
         <v>3.5</v>
       </c>
@@ -3164,33 +3250,33 @@
       <c r="AF34" s="5"/>
     </row>
     <row r="35" ht="15.0" customHeight="1">
-      <c r="A35" s="107" t="s">
+      <c r="A35" s="105" t="s">
+        <v>78</v>
+      </c>
+      <c r="B35" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="B35" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="C35" s="108"/>
+      <c r="C35" s="106"/>
       <c r="D35" s="70"/>
       <c r="E35" s="71"/>
-      <c r="F35" s="102"/>
-      <c r="G35" s="109">
+      <c r="F35" s="100"/>
+      <c r="G35" s="107">
         <f>SUM(F36:F40)</f>
         <v>15.5</v>
       </c>
-      <c r="H35" s="102"/>
-      <c r="I35" s="110">
+      <c r="H35" s="100"/>
+      <c r="I35" s="108">
         <f>SUM(H36:H40)</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J35" s="6"/>
       <c r="K35" s="6"/>
       <c r="L35" s="6"/>
-      <c r="M35" s="111"/>
-      <c r="N35" s="111"/>
-      <c r="O35" s="111"/>
-      <c r="P35" s="111"/>
-      <c r="Q35" s="111">
+      <c r="M35" s="109"/>
+      <c r="N35" s="109"/>
+      <c r="O35" s="109"/>
+      <c r="P35" s="109"/>
+      <c r="Q35" s="109">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3211,10 +3297,10 @@
       <c r="AF35" s="6"/>
     </row>
     <row r="36" ht="15.0" customHeight="1">
-      <c r="A36" s="107"/>
-      <c r="B36" s="112"/>
+      <c r="A36" s="105"/>
+      <c r="B36" s="110"/>
       <c r="C36" s="40" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D36" s="41" t="s">
         <v>20</v>
@@ -3225,24 +3311,32 @@
       <c r="F36" s="43">
         <v>3.0</v>
       </c>
-      <c r="G36" s="113"/>
+      <c r="G36" s="111"/>
       <c r="H36" s="45">
         <f t="shared" ref="H36:H40" si="6">SUM(M36:P36)</f>
-        <v>0</v>
-      </c>
-      <c r="I36" s="113"/>
-      <c r="J36" s="84" t="s">
-        <v>67</v>
+        <v>1.5</v>
+      </c>
+      <c r="I36" s="111"/>
+      <c r="J36" s="82" t="s">
+        <v>81</v>
       </c>
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
-      <c r="M36" s="114"/>
-      <c r="N36" s="115"/>
-      <c r="O36" s="115"/>
-      <c r="P36" s="115"/>
-      <c r="Q36" s="115">
+      <c r="M36" s="112">
+        <v>0.5</v>
+      </c>
+      <c r="N36" s="112">
+        <v>0.5</v>
+      </c>
+      <c r="O36" s="112">
+        <v>0.5</v>
+      </c>
+      <c r="P36" s="112" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q36" s="113">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="R36" s="5"/>
       <c r="S36" s="5"/>
@@ -3261,10 +3355,10 @@
       <c r="AF36" s="5"/>
     </row>
     <row r="37" ht="15.0" customHeight="1">
-      <c r="A37" s="107"/>
-      <c r="B37" s="112"/>
+      <c r="A37" s="105"/>
+      <c r="B37" s="110"/>
       <c r="C37" s="40" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D37" s="41" t="s">
         <v>20</v>
@@ -3275,32 +3369,32 @@
       <c r="F37" s="43">
         <v>4.0</v>
       </c>
-      <c r="G37" s="113"/>
+      <c r="G37" s="111"/>
       <c r="H37" s="45">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="I37" s="113"/>
-      <c r="J37" s="84" t="s">
-        <v>67</v>
+        <v>3.5</v>
+      </c>
+      <c r="I37" s="111"/>
+      <c r="J37" s="82" t="s">
+        <v>57</v>
       </c>
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
-      <c r="M37" s="114">
+      <c r="M37" s="112">
+        <v>1.0</v>
+      </c>
+      <c r="N37" s="112">
+        <v>1.0</v>
+      </c>
+      <c r="O37" s="112">
+        <v>1.0</v>
+      </c>
+      <c r="P37" s="112">
         <v>0.5</v>
       </c>
-      <c r="N37" s="114" t="s">
-        <v>83</v>
-      </c>
-      <c r="O37" s="114">
-        <v>0.5</v>
-      </c>
-      <c r="P37" s="114" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q37" s="115">
+      <c r="Q37" s="113">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3.5</v>
       </c>
       <c r="R37" s="5"/>
       <c r="S37" s="5"/>
@@ -3319,9 +3413,9 @@
       <c r="AF37" s="5"/>
     </row>
     <row r="38" ht="33.75" customHeight="1">
-      <c r="A38" s="107"/>
-      <c r="B38" s="112"/>
-      <c r="C38" s="116" t="s">
+      <c r="A38" s="105"/>
+      <c r="B38" s="110"/>
+      <c r="C38" s="114" t="s">
         <v>84</v>
       </c>
       <c r="D38" s="41" t="s">
@@ -3333,22 +3427,30 @@
       <c r="F38" s="43">
         <v>2.5</v>
       </c>
-      <c r="G38" s="113"/>
+      <c r="G38" s="111"/>
       <c r="H38" s="45">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="I38" s="113"/>
-      <c r="J38" s="84" t="s">
+      <c r="I38" s="111"/>
+      <c r="J38" s="85" t="s">
         <v>67</v>
       </c>
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
-      <c r="M38" s="115"/>
-      <c r="N38" s="115"/>
-      <c r="O38" s="115"/>
-      <c r="P38" s="114"/>
-      <c r="Q38" s="115">
+      <c r="M38" s="112" t="s">
+        <v>82</v>
+      </c>
+      <c r="N38" s="112" t="s">
+        <v>82</v>
+      </c>
+      <c r="O38" s="112" t="s">
+        <v>82</v>
+      </c>
+      <c r="P38" s="112" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q38" s="113">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3369,36 +3471,44 @@
       <c r="AF38" s="5"/>
     </row>
     <row r="39" ht="31.5" customHeight="1">
-      <c r="A39" s="107"/>
-      <c r="B39" s="112"/>
-      <c r="C39" s="116" t="s">
+      <c r="A39" s="105"/>
+      <c r="B39" s="110"/>
+      <c r="C39" s="114" t="s">
         <v>86</v>
       </c>
       <c r="D39" s="41" t="s">
         <v>52</v>
       </c>
       <c r="E39" s="42" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F39" s="43">
         <v>4.0</v>
       </c>
-      <c r="G39" s="113"/>
+      <c r="G39" s="111"/>
       <c r="H39" s="45">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="I39" s="113"/>
-      <c r="J39" s="84" t="s">
+      <c r="I39" s="111"/>
+      <c r="J39" s="85" t="s">
         <v>67</v>
       </c>
       <c r="K39" s="5"/>
       <c r="L39" s="5"/>
-      <c r="M39" s="115"/>
-      <c r="N39" s="115"/>
-      <c r="O39" s="115"/>
-      <c r="P39" s="115"/>
-      <c r="Q39" s="115">
+      <c r="M39" s="112" t="s">
+        <v>82</v>
+      </c>
+      <c r="N39" s="112" t="s">
+        <v>82</v>
+      </c>
+      <c r="O39" s="112" t="s">
+        <v>82</v>
+      </c>
+      <c r="P39" s="112" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q39" s="113">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3419,38 +3529,46 @@
       <c r="AF39" s="5"/>
     </row>
     <row r="40" ht="15.0" customHeight="1">
-      <c r="A40" s="107"/>
-      <c r="B40" s="117"/>
-      <c r="C40" s="118" t="s">
-        <v>87</v>
+      <c r="A40" s="105"/>
+      <c r="B40" s="115"/>
+      <c r="C40" s="116" t="s">
+        <v>88</v>
       </c>
       <c r="D40" s="52" t="s">
         <v>52</v>
       </c>
       <c r="E40" s="53" t="s">
-        <v>60</v>
-      </c>
-      <c r="F40" s="119">
+        <v>61</v>
+      </c>
+      <c r="F40" s="117">
         <v>2.0</v>
       </c>
-      <c r="G40" s="120"/>
+      <c r="G40" s="118"/>
       <c r="H40" s="56">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="I40" s="120"/>
-      <c r="J40" s="84" t="s">
-        <v>67</v>
+        <v>2</v>
+      </c>
+      <c r="I40" s="118"/>
+      <c r="J40" s="82" t="s">
+        <v>54</v>
       </c>
       <c r="K40" s="5"/>
       <c r="L40" s="5"/>
-      <c r="M40" s="121"/>
-      <c r="N40" s="121"/>
-      <c r="O40" s="121"/>
-      <c r="P40" s="122"/>
-      <c r="Q40" s="121">
+      <c r="M40" s="119">
+        <v>0.5</v>
+      </c>
+      <c r="N40" s="119">
+        <v>0.75</v>
+      </c>
+      <c r="O40" s="119">
+        <v>0.75</v>
+      </c>
+      <c r="P40" s="119" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q40" s="120">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R40" s="5"/>
       <c r="S40" s="5"/>
@@ -3469,31 +3587,31 @@
       <c r="AF40" s="5"/>
     </row>
     <row r="41" ht="15.0" customHeight="1">
-      <c r="A41" s="107"/>
+      <c r="A41" s="105"/>
       <c r="B41" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="C41" s="108"/>
+      <c r="C41" s="106"/>
       <c r="D41" s="70"/>
       <c r="E41" s="71"/>
-      <c r="F41" s="102"/>
-      <c r="G41" s="109">
+      <c r="F41" s="100"/>
+      <c r="G41" s="107">
         <f>SUM(F42:F46)</f>
         <v>11</v>
       </c>
-      <c r="H41" s="102"/>
-      <c r="I41" s="110">
+      <c r="H41" s="100"/>
+      <c r="I41" s="108">
         <f>SUM(H42:H46)</f>
-        <v>0</v>
+        <v>6.4</v>
       </c>
       <c r="J41" s="5"/>
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
-      <c r="M41" s="111"/>
-      <c r="N41" s="111"/>
-      <c r="O41" s="111"/>
-      <c r="P41" s="111"/>
-      <c r="Q41" s="111">
+      <c r="M41" s="109"/>
+      <c r="N41" s="109"/>
+      <c r="O41" s="109"/>
+      <c r="P41" s="109"/>
+      <c r="Q41" s="109">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3514,38 +3632,46 @@
       <c r="AF41" s="5"/>
     </row>
     <row r="42" ht="27.0" customHeight="1">
-      <c r="A42" s="107"/>
-      <c r="B42" s="112"/>
+      <c r="A42" s="105"/>
+      <c r="B42" s="110"/>
       <c r="C42" s="40" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D42" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="E42" s="123" t="s">
-        <v>89</v>
+      <c r="E42" s="42" t="s">
+        <v>90</v>
       </c>
       <c r="F42" s="43">
         <v>4.0</v>
       </c>
-      <c r="G42" s="113"/>
+      <c r="G42" s="111"/>
       <c r="H42" s="45">
         <f t="shared" ref="H42:H46" si="7">SUM(M42:P42)</f>
-        <v>0</v>
-      </c>
-      <c r="I42" s="113"/>
-      <c r="J42" s="84" t="s">
-        <v>67</v>
+        <v>4.6</v>
+      </c>
+      <c r="I42" s="111"/>
+      <c r="J42" s="82" t="s">
+        <v>57</v>
       </c>
       <c r="K42" s="5"/>
       <c r="L42" s="5"/>
-      <c r="M42" s="115"/>
-      <c r="N42" s="115"/>
-      <c r="O42" s="114"/>
-      <c r="P42" s="114"/>
-      <c r="Q42" s="115">
+      <c r="M42" s="112">
+        <v>1.2</v>
+      </c>
+      <c r="N42" s="112">
+        <v>1.2</v>
+      </c>
+      <c r="O42" s="112">
+        <v>1.2</v>
+      </c>
+      <c r="P42" s="112">
+        <v>1.0</v>
+      </c>
+      <c r="Q42" s="113">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4.6</v>
       </c>
       <c r="R42" s="5"/>
       <c r="S42" s="5"/>
@@ -3564,38 +3690,46 @@
       <c r="AF42" s="5"/>
     </row>
     <row r="43" ht="15.0" customHeight="1">
-      <c r="A43" s="107"/>
-      <c r="B43" s="112"/>
-      <c r="C43" s="116" t="s">
-        <v>90</v>
+      <c r="A43" s="105"/>
+      <c r="B43" s="110"/>
+      <c r="C43" s="114" t="s">
+        <v>91</v>
       </c>
       <c r="D43" s="41" t="s">
         <v>52</v>
       </c>
       <c r="E43" s="42" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F43" s="43">
         <v>2.5</v>
       </c>
-      <c r="G43" s="113"/>
+      <c r="G43" s="111"/>
       <c r="H43" s="45">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="I43" s="113"/>
-      <c r="J43" s="84" t="s">
-        <v>67</v>
+        <v>0.8</v>
+      </c>
+      <c r="I43" s="111"/>
+      <c r="J43" s="82" t="s">
+        <v>81</v>
       </c>
       <c r="K43" s="5"/>
       <c r="L43" s="5"/>
-      <c r="M43" s="115"/>
-      <c r="N43" s="115"/>
-      <c r="O43" s="114"/>
-      <c r="P43" s="115"/>
-      <c r="Q43" s="115">
+      <c r="M43" s="112">
+        <v>0.8</v>
+      </c>
+      <c r="N43" s="112" t="s">
+        <v>82</v>
+      </c>
+      <c r="O43" s="112" t="s">
+        <v>82</v>
+      </c>
+      <c r="P43" s="112" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q43" s="113">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="R43" s="5"/>
       <c r="S43" s="5"/>
@@ -3613,37 +3747,45 @@
       <c r="AE43" s="5"/>
       <c r="AF43" s="5"/>
     </row>
-    <row r="44" ht="29.25" customHeight="1">
-      <c r="A44" s="107"/>
-      <c r="B44" s="112"/>
-      <c r="C44" s="116" t="s">
-        <v>92</v>
+    <row r="44" ht="20.25" customHeight="1">
+      <c r="A44" s="105"/>
+      <c r="B44" s="110"/>
+      <c r="C44" s="114" t="s">
+        <v>93</v>
       </c>
       <c r="D44" s="41" t="s">
         <v>52</v>
       </c>
       <c r="E44" s="42" t="s">
-        <v>93</v>
+        <v>66</v>
       </c>
       <c r="F44" s="43">
         <v>1.0</v>
       </c>
-      <c r="G44" s="113"/>
+      <c r="G44" s="111"/>
       <c r="H44" s="45">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I44" s="113"/>
-      <c r="J44" s="84" t="s">
+      <c r="I44" s="111"/>
+      <c r="J44" s="85" t="s">
         <v>67</v>
       </c>
       <c r="K44" s="5"/>
       <c r="L44" s="5"/>
-      <c r="M44" s="114"/>
-      <c r="N44" s="115"/>
-      <c r="O44" s="114"/>
-      <c r="P44" s="115"/>
-      <c r="Q44" s="115">
+      <c r="M44" s="112" t="s">
+        <v>82</v>
+      </c>
+      <c r="N44" s="112" t="s">
+        <v>82</v>
+      </c>
+      <c r="O44" s="112" t="s">
+        <v>82</v>
+      </c>
+      <c r="P44" s="112" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q44" s="113">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3664,36 +3806,44 @@
       <c r="AF44" s="5"/>
     </row>
     <row r="45" ht="15.0" customHeight="1">
-      <c r="A45" s="107"/>
-      <c r="B45" s="112"/>
-      <c r="C45" s="116" t="s">
+      <c r="A45" s="105"/>
+      <c r="B45" s="110"/>
+      <c r="C45" s="114" t="s">
         <v>94</v>
       </c>
       <c r="D45" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="E45" s="124" t="s">
-        <v>60</v>
+      <c r="E45" s="42" t="s">
+        <v>61</v>
       </c>
       <c r="F45" s="43">
         <v>2.0</v>
       </c>
-      <c r="G45" s="113"/>
+      <c r="G45" s="111"/>
       <c r="H45" s="45">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I45" s="113"/>
-      <c r="J45" s="84" t="s">
+      <c r="I45" s="111"/>
+      <c r="J45" s="85" t="s">
         <v>67</v>
       </c>
       <c r="K45" s="5"/>
       <c r="L45" s="5"/>
-      <c r="M45" s="115"/>
-      <c r="N45" s="115"/>
-      <c r="O45" s="114"/>
-      <c r="P45" s="114"/>
-      <c r="Q45" s="115">
+      <c r="M45" s="112" t="s">
+        <v>82</v>
+      </c>
+      <c r="N45" s="112" t="s">
+        <v>82</v>
+      </c>
+      <c r="O45" s="112" t="s">
+        <v>82</v>
+      </c>
+      <c r="P45" s="112" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q45" s="113">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3714,8 +3864,8 @@
       <c r="AF45" s="5"/>
     </row>
     <row r="46" ht="15.0" customHeight="1">
-      <c r="A46" s="107"/>
-      <c r="B46" s="117"/>
+      <c r="A46" s="105"/>
+      <c r="B46" s="115"/>
       <c r="C46" s="51" t="s">
         <v>69</v>
       </c>
@@ -3725,27 +3875,35 @@
       <c r="E46" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="F46" s="119">
+      <c r="F46" s="117">
         <v>1.5</v>
       </c>
-      <c r="G46" s="120"/>
+      <c r="G46" s="118"/>
       <c r="H46" s="56">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="I46" s="120"/>
-      <c r="J46" s="84" t="s">
-        <v>67</v>
+        <v>1</v>
+      </c>
+      <c r="I46" s="118"/>
+      <c r="J46" s="82" t="s">
+        <v>54</v>
       </c>
       <c r="K46" s="5"/>
       <c r="L46" s="5"/>
-      <c r="M46" s="121"/>
-      <c r="N46" s="121"/>
-      <c r="O46" s="122"/>
-      <c r="P46" s="121"/>
-      <c r="Q46" s="121">
+      <c r="M46" s="119">
+        <v>0.5</v>
+      </c>
+      <c r="N46" s="119" t="s">
+        <v>82</v>
+      </c>
+      <c r="O46" s="119">
+        <v>0.5</v>
+      </c>
+      <c r="P46" s="119" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q46" s="120">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R46" s="5"/>
       <c r="S46" s="5"/>
@@ -3764,31 +3922,31 @@
       <c r="AF46" s="5"/>
     </row>
     <row r="47" ht="15.0" customHeight="1">
-      <c r="A47" s="107"/>
+      <c r="A47" s="105"/>
       <c r="B47" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="C47" s="108"/>
+      <c r="C47" s="106"/>
       <c r="D47" s="70"/>
       <c r="E47" s="71"/>
-      <c r="F47" s="102"/>
-      <c r="G47" s="109">
+      <c r="F47" s="100"/>
+      <c r="G47" s="107">
         <f>SUM(F48:F50)</f>
         <v>7</v>
       </c>
-      <c r="H47" s="102"/>
-      <c r="I47" s="110">
+      <c r="H47" s="100"/>
+      <c r="I47" s="108">
         <f>SUM(H48:H50)</f>
-        <v>0</v>
+        <v>4.7</v>
       </c>
       <c r="J47" s="5"/>
       <c r="K47" s="5"/>
       <c r="L47" s="5"/>
-      <c r="M47" s="111"/>
-      <c r="N47" s="111"/>
-      <c r="O47" s="111"/>
-      <c r="P47" s="111"/>
-      <c r="Q47" s="111">
+      <c r="M47" s="109"/>
+      <c r="N47" s="109"/>
+      <c r="O47" s="109"/>
+      <c r="P47" s="109"/>
+      <c r="Q47" s="109">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3809,38 +3967,46 @@
       <c r="AF47" s="5"/>
     </row>
     <row r="48" ht="15.0" customHeight="1">
-      <c r="A48" s="107"/>
-      <c r="B48" s="112"/>
-      <c r="C48" s="125" t="s">
+      <c r="A48" s="105"/>
+      <c r="B48" s="110"/>
+      <c r="C48" s="121" t="s">
         <v>72</v>
       </c>
       <c r="D48" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="E48" s="123" t="s">
-        <v>60</v>
+      <c r="E48" s="122" t="s">
+        <v>61</v>
       </c>
       <c r="F48" s="43">
         <v>2.0</v>
       </c>
-      <c r="G48" s="113"/>
+      <c r="G48" s="111"/>
       <c r="H48" s="45">
         <f t="shared" ref="H48:H50" si="8">SUM(M48:P48)</f>
-        <v>0</v>
-      </c>
-      <c r="I48" s="113"/>
-      <c r="J48" s="84" t="s">
-        <v>67</v>
+        <v>1.5</v>
+      </c>
+      <c r="I48" s="111"/>
+      <c r="J48" s="82" t="s">
+        <v>81</v>
       </c>
       <c r="K48" s="5"/>
       <c r="L48" s="5"/>
-      <c r="M48" s="114"/>
-      <c r="N48" s="114"/>
-      <c r="O48" s="115"/>
-      <c r="P48" s="115"/>
-      <c r="Q48" s="115">
+      <c r="M48" s="112">
+        <v>0.5</v>
+      </c>
+      <c r="N48" s="112" t="s">
+        <v>82</v>
+      </c>
+      <c r="O48" s="112">
+        <v>1.0</v>
+      </c>
+      <c r="P48" s="112" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q48" s="113">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="R48" s="5"/>
       <c r="S48" s="5"/>
@@ -3859,36 +4025,44 @@
       <c r="AF48" s="5"/>
     </row>
     <row r="49" ht="15.0" customHeight="1">
-      <c r="A49" s="107"/>
-      <c r="B49" s="112"/>
+      <c r="A49" s="105"/>
+      <c r="B49" s="110"/>
       <c r="C49" s="40" t="s">
         <v>96</v>
       </c>
       <c r="D49" s="41" t="s">
-        <v>75</v>
-      </c>
-      <c r="E49" s="126" t="s">
+        <v>74</v>
+      </c>
+      <c r="E49" s="123" t="s">
         <v>97</v>
       </c>
       <c r="F49" s="43">
         <v>2.0</v>
       </c>
-      <c r="G49" s="113"/>
+      <c r="G49" s="111"/>
       <c r="H49" s="45">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="I49" s="113"/>
-      <c r="J49" s="84" t="s">
-        <v>67</v>
+      <c r="I49" s="111"/>
+      <c r="J49" s="82" t="s">
+        <v>76</v>
       </c>
       <c r="K49" s="5"/>
       <c r="L49" s="5"/>
-      <c r="M49" s="114"/>
-      <c r="N49" s="115"/>
-      <c r="O49" s="114"/>
-      <c r="P49" s="114"/>
-      <c r="Q49" s="115">
+      <c r="M49" s="112">
+        <v>0.0</v>
+      </c>
+      <c r="N49" s="112">
+        <v>0.0</v>
+      </c>
+      <c r="O49" s="112">
+        <v>0.0</v>
+      </c>
+      <c r="P49" s="112">
+        <v>0.0</v>
+      </c>
+      <c r="Q49" s="113">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3909,38 +4083,46 @@
       <c r="AF49" s="5"/>
     </row>
     <row r="50" ht="15.0" customHeight="1">
-      <c r="A50" s="107"/>
-      <c r="B50" s="117"/>
+      <c r="A50" s="105"/>
+      <c r="B50" s="115"/>
       <c r="C50" s="51" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D50" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="E50" s="127" t="s">
+      <c r="E50" s="124" t="s">
         <v>21</v>
       </c>
-      <c r="F50" s="119">
+      <c r="F50" s="117">
         <v>3.0</v>
       </c>
-      <c r="G50" s="120"/>
+      <c r="G50" s="118"/>
       <c r="H50" s="56">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="I50" s="120"/>
-      <c r="J50" s="84" t="s">
-        <v>67</v>
+        <v>3.2</v>
+      </c>
+      <c r="I50" s="118"/>
+      <c r="J50" s="82" t="s">
+        <v>57</v>
       </c>
       <c r="K50" s="5"/>
       <c r="L50" s="5"/>
-      <c r="M50" s="122"/>
-      <c r="N50" s="121"/>
-      <c r="O50" s="121"/>
-      <c r="P50" s="121"/>
-      <c r="Q50" s="121">
+      <c r="M50" s="119">
+        <v>1.2</v>
+      </c>
+      <c r="N50" s="119">
+        <v>1.2</v>
+      </c>
+      <c r="O50" s="119">
+        <v>0.5</v>
+      </c>
+      <c r="P50" s="119">
+        <v>0.3</v>
+      </c>
+      <c r="Q50" s="120">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.2</v>
       </c>
       <c r="R50" s="5"/>
       <c r="S50" s="5"/>
@@ -3963,29 +4145,29 @@
         <v>98</v>
       </c>
       <c r="B51" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="C51" s="108"/>
+        <v>79</v>
+      </c>
+      <c r="C51" s="106"/>
       <c r="D51" s="70"/>
       <c r="E51" s="71"/>
       <c r="F51" s="72"/>
-      <c r="G51" s="109">
+      <c r="G51" s="107">
         <f>SUM(F52:F55)</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="H51" s="72"/>
-      <c r="I51" s="110">
+      <c r="I51" s="108">
         <f>SUM(H52:H55)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J51" s="6"/>
       <c r="K51" s="6"/>
       <c r="L51" s="6"/>
-      <c r="M51" s="111"/>
-      <c r="N51" s="111"/>
-      <c r="O51" s="111"/>
-      <c r="P51" s="111"/>
-      <c r="Q51" s="111">
+      <c r="M51" s="109"/>
+      <c r="N51" s="109"/>
+      <c r="O51" s="109"/>
+      <c r="P51" s="109"/>
+      <c r="Q51" s="109">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4006,34 +4188,40 @@
       <c r="AF51" s="6"/>
     </row>
     <row r="52" ht="15.0" customHeight="1">
-      <c r="A52" s="128"/>
-      <c r="B52" s="129"/>
+      <c r="A52" s="125"/>
+      <c r="B52" s="126"/>
       <c r="C52" s="60" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D52" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="E52" s="130"/>
-      <c r="F52" s="131" t="s">
-        <v>83</v>
-      </c>
-      <c r="G52" s="132"/>
+      <c r="E52" s="127" t="s">
+        <v>21</v>
+      </c>
+      <c r="F52" s="128">
+        <v>2.0</v>
+      </c>
+      <c r="G52" s="129"/>
       <c r="H52" s="65">
         <f t="shared" ref="H52:H55" si="9">SUM(M52:P52)</f>
-        <v>0</v>
-      </c>
-      <c r="I52" s="133"/>
-      <c r="J52" s="5"/>
+        <v>0.1</v>
+      </c>
+      <c r="I52" s="130"/>
+      <c r="J52" s="82" t="s">
+        <v>54</v>
+      </c>
       <c r="K52" s="5"/>
       <c r="L52" s="5"/>
-      <c r="M52" s="134"/>
-      <c r="N52" s="135"/>
-      <c r="O52" s="135"/>
-      <c r="P52" s="135"/>
-      <c r="Q52" s="135">
+      <c r="M52" s="131">
+        <v>0.1</v>
+      </c>
+      <c r="N52" s="132"/>
+      <c r="O52" s="132"/>
+      <c r="P52" s="132"/>
+      <c r="Q52" s="132">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="R52" s="5"/>
       <c r="S52" s="5"/>
@@ -4053,33 +4241,43 @@
     </row>
     <row r="53" ht="15.0" customHeight="1">
       <c r="A53" s="68"/>
-      <c r="B53" s="89"/>
-      <c r="C53" s="136" t="s">
-        <v>82</v>
+      <c r="B53" s="88"/>
+      <c r="C53" s="133" t="s">
+        <v>83</v>
       </c>
       <c r="D53" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="E53" s="137"/>
-      <c r="F53" s="138" t="s">
-        <v>83</v>
+      <c r="E53" s="134" t="s">
+        <v>99</v>
+      </c>
+      <c r="F53" s="135">
+        <v>4.0</v>
       </c>
       <c r="G53" s="79"/>
-      <c r="H53" s="139">
+      <c r="H53" s="136">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="I53" s="79"/>
-      <c r="J53" s="5"/>
+      <c r="J53" s="82" t="s">
+        <v>54</v>
+      </c>
       <c r="K53" s="5"/>
       <c r="L53" s="5"/>
-      <c r="M53" s="104"/>
-      <c r="N53" s="104"/>
-      <c r="O53" s="105"/>
-      <c r="P53" s="105"/>
-      <c r="Q53" s="105">
+      <c r="M53" s="137">
+        <v>0.3</v>
+      </c>
+      <c r="N53" s="137">
+        <v>0.3</v>
+      </c>
+      <c r="O53" s="137">
+        <v>0.3</v>
+      </c>
+      <c r="P53" s="103"/>
+      <c r="Q53" s="103">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="R53" s="5"/>
       <c r="S53" s="5"/>
@@ -4099,35 +4297,49 @@
     </row>
     <row r="54" ht="15.0" customHeight="1">
       <c r="A54" s="68"/>
-      <c r="B54" s="89"/>
-      <c r="C54" s="136" t="s">
-        <v>99</v>
+      <c r="B54" s="88"/>
+      <c r="C54" s="138" t="s">
+        <v>88</v>
       </c>
       <c r="D54" s="76" t="s">
         <v>52</v>
       </c>
-      <c r="E54" s="140"/>
-      <c r="F54" s="138" t="s">
-        <v>83</v>
+      <c r="E54" s="139" t="s">
+        <v>61</v>
+      </c>
+      <c r="F54" s="135">
+        <v>4.0</v>
       </c>
       <c r="G54" s="79"/>
-      <c r="H54" s="139">
+      <c r="H54" s="136">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I54" s="79"/>
-      <c r="J54" s="5"/>
+      <c r="J54" s="82" t="s">
+        <v>54</v>
+      </c>
       <c r="K54" s="5"/>
       <c r="L54" s="5"/>
-      <c r="M54" s="104"/>
-      <c r="N54" s="105"/>
-      <c r="O54" s="105"/>
-      <c r="P54" s="104"/>
-      <c r="Q54" s="105">
+      <c r="M54" s="137" t="s">
+        <v>82</v>
+      </c>
+      <c r="N54" s="137" t="s">
+        <v>82</v>
+      </c>
+      <c r="O54" s="137" t="s">
+        <v>82</v>
+      </c>
+      <c r="P54" s="137" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q54" s="103">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R54" s="5"/>
+      <c r="R54" s="82" t="s">
+        <v>100</v>
+      </c>
       <c r="S54" s="5"/>
       <c r="T54" s="5"/>
       <c r="U54" s="5"/>
@@ -4143,37 +4355,43 @@
       <c r="AE54" s="5"/>
       <c r="AF54" s="5"/>
     </row>
-    <row r="55" ht="15.0" customHeight="1">
+    <row r="55" ht="35.25" customHeight="1">
       <c r="A55" s="68"/>
-      <c r="B55" s="90"/>
-      <c r="C55" s="141" t="s">
-        <v>100</v>
-      </c>
-      <c r="D55" s="92" t="s">
+      <c r="B55" s="89"/>
+      <c r="C55" s="140" t="s">
+        <v>101</v>
+      </c>
+      <c r="D55" s="91" t="s">
         <v>52</v>
       </c>
-      <c r="E55" s="142"/>
-      <c r="F55" s="143" t="s">
-        <v>83</v>
-      </c>
-      <c r="G55" s="95"/>
-      <c r="H55" s="144">
+      <c r="E55" s="141" t="s">
+        <v>64</v>
+      </c>
+      <c r="F55" s="142">
+        <v>3.0</v>
+      </c>
+      <c r="G55" s="94"/>
+      <c r="H55" s="143">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="I55" s="95"/>
-      <c r="J55" s="5"/>
+      <c r="I55" s="94"/>
+      <c r="J55" s="82" t="s">
+        <v>67</v>
+      </c>
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
-      <c r="M55" s="145"/>
-      <c r="N55" s="146"/>
-      <c r="O55" s="146"/>
-      <c r="P55" s="146"/>
-      <c r="Q55" s="146">
+      <c r="M55" s="144"/>
+      <c r="N55" s="145"/>
+      <c r="O55" s="145"/>
+      <c r="P55" s="145"/>
+      <c r="Q55" s="145">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R55" s="5"/>
+      <c r="R55" s="82" t="s">
+        <v>100</v>
+      </c>
       <c r="S55" s="5"/>
       <c r="T55" s="5"/>
       <c r="U55" s="5"/>
@@ -4194,27 +4412,27 @@
       <c r="B56" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="C56" s="108"/>
+      <c r="C56" s="106"/>
       <c r="D56" s="70"/>
       <c r="E56" s="71"/>
-      <c r="F56" s="102"/>
-      <c r="G56" s="109">
+      <c r="F56" s="100"/>
+      <c r="G56" s="107">
         <f>SUM(F57:F61)</f>
-        <v>0</v>
-      </c>
-      <c r="H56" s="102"/>
-      <c r="I56" s="110">
+        <v>18.5</v>
+      </c>
+      <c r="H56" s="100"/>
+      <c r="I56" s="108">
         <f>SUM(H57:H61)</f>
         <v>0</v>
       </c>
       <c r="J56" s="5"/>
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
-      <c r="M56" s="111"/>
-      <c r="N56" s="111"/>
-      <c r="O56" s="111"/>
-      <c r="P56" s="111"/>
-      <c r="Q56" s="111">
+      <c r="M56" s="109"/>
+      <c r="N56" s="109"/>
+      <c r="O56" s="109"/>
+      <c r="P56" s="109"/>
+      <c r="Q56" s="109">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4236,31 +4454,35 @@
     </row>
     <row r="57" ht="15.0" customHeight="1">
       <c r="A57" s="68"/>
-      <c r="B57" s="89"/>
-      <c r="C57" s="136" t="s">
-        <v>88</v>
+      <c r="B57" s="88"/>
+      <c r="C57" s="133" t="s">
+        <v>89</v>
       </c>
       <c r="D57" s="76" t="s">
         <v>52</v>
       </c>
-      <c r="E57" s="140"/>
-      <c r="F57" s="138" t="s">
-        <v>83</v>
+      <c r="E57" s="139" t="s">
+        <v>64</v>
+      </c>
+      <c r="F57" s="135">
+        <v>4.0</v>
       </c>
       <c r="G57" s="79"/>
-      <c r="H57" s="139">
+      <c r="H57" s="136">
         <f t="shared" ref="H57:H61" si="10">SUM(M57:P57)</f>
         <v>0</v>
       </c>
       <c r="I57" s="79"/>
-      <c r="J57" s="5"/>
+      <c r="J57" s="82" t="s">
+        <v>67</v>
+      </c>
       <c r="K57" s="5"/>
       <c r="L57" s="5"/>
-      <c r="M57" s="105"/>
-      <c r="N57" s="105"/>
-      <c r="O57" s="105"/>
-      <c r="P57" s="105"/>
-      <c r="Q57" s="105">
+      <c r="M57" s="103"/>
+      <c r="N57" s="103"/>
+      <c r="O57" s="103"/>
+      <c r="P57" s="103"/>
+      <c r="Q57" s="103">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4282,31 +4504,35 @@
     </row>
     <row r="58" ht="29.25" customHeight="1">
       <c r="A58" s="68"/>
-      <c r="B58" s="89"/>
-      <c r="C58" s="136" t="s">
-        <v>101</v>
+      <c r="B58" s="88"/>
+      <c r="C58" s="146" t="s">
+        <v>102</v>
       </c>
       <c r="D58" s="76" t="s">
         <v>52</v>
       </c>
-      <c r="E58" s="140"/>
-      <c r="F58" s="138" t="s">
-        <v>83</v>
+      <c r="E58" s="134" t="s">
+        <v>103</v>
+      </c>
+      <c r="F58" s="135">
+        <v>3.0</v>
       </c>
       <c r="G58" s="79"/>
-      <c r="H58" s="139">
+      <c r="H58" s="136">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I58" s="79"/>
-      <c r="J58" s="5"/>
+      <c r="J58" s="82" t="s">
+        <v>67</v>
+      </c>
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
-      <c r="M58" s="105"/>
-      <c r="N58" s="105"/>
-      <c r="O58" s="105"/>
-      <c r="P58" s="104"/>
-      <c r="Q58" s="105">
+      <c r="M58" s="103"/>
+      <c r="N58" s="103"/>
+      <c r="O58" s="103"/>
+      <c r="P58" s="102"/>
+      <c r="Q58" s="103">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4328,31 +4554,35 @@
     </row>
     <row r="59" ht="15.0" customHeight="1">
       <c r="A59" s="68"/>
-      <c r="B59" s="89"/>
-      <c r="C59" s="136" t="s">
-        <v>102</v>
+      <c r="B59" s="88"/>
+      <c r="C59" s="146" t="s">
+        <v>104</v>
       </c>
       <c r="D59" s="76" t="s">
         <v>52</v>
       </c>
-      <c r="E59" s="140"/>
-      <c r="F59" s="138" t="s">
-        <v>83</v>
+      <c r="E59" s="139" t="s">
+        <v>66</v>
+      </c>
+      <c r="F59" s="135">
+        <v>6.0</v>
       </c>
       <c r="G59" s="79"/>
-      <c r="H59" s="139">
+      <c r="H59" s="136">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I59" s="79"/>
-      <c r="J59" s="5"/>
+      <c r="J59" s="82" t="s">
+        <v>67</v>
+      </c>
       <c r="K59" s="5"/>
       <c r="L59" s="5"/>
-      <c r="M59" s="105"/>
-      <c r="N59" s="105"/>
-      <c r="O59" s="105"/>
-      <c r="P59" s="104"/>
-      <c r="Q59" s="105">
+      <c r="M59" s="103"/>
+      <c r="N59" s="103"/>
+      <c r="O59" s="103"/>
+      <c r="P59" s="102"/>
+      <c r="Q59" s="103">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4374,31 +4604,35 @@
     </row>
     <row r="60" ht="15.0" customHeight="1">
       <c r="A60" s="68"/>
-      <c r="B60" s="89"/>
-      <c r="C60" s="136" t="s">
-        <v>103</v>
+      <c r="B60" s="88"/>
+      <c r="C60" s="146" t="s">
+        <v>105</v>
       </c>
       <c r="D60" s="76" t="s">
         <v>52</v>
       </c>
-      <c r="E60" s="140"/>
-      <c r="F60" s="138" t="s">
-        <v>83</v>
+      <c r="E60" s="139" t="s">
+        <v>64</v>
+      </c>
+      <c r="F60" s="135">
+        <v>4.0</v>
       </c>
       <c r="G60" s="79"/>
-      <c r="H60" s="139">
+      <c r="H60" s="136">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I60" s="79"/>
-      <c r="J60" s="5"/>
+      <c r="J60" s="82" t="s">
+        <v>67</v>
+      </c>
       <c r="K60" s="5"/>
       <c r="L60" s="5"/>
-      <c r="M60" s="105"/>
-      <c r="N60" s="105"/>
-      <c r="O60" s="105"/>
-      <c r="P60" s="104"/>
-      <c r="Q60" s="105">
+      <c r="M60" s="103"/>
+      <c r="N60" s="103"/>
+      <c r="O60" s="103"/>
+      <c r="P60" s="102"/>
+      <c r="Q60" s="103">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4420,31 +4654,35 @@
     </row>
     <row r="61" ht="15.0" customHeight="1">
       <c r="A61" s="68"/>
-      <c r="B61" s="90"/>
-      <c r="C61" s="141" t="s">
+      <c r="B61" s="89"/>
+      <c r="C61" s="147" t="s">
         <v>69</v>
       </c>
-      <c r="D61" s="92" t="s">
+      <c r="D61" s="91" t="s">
         <v>52</v>
       </c>
-      <c r="E61" s="142"/>
-      <c r="F61" s="143" t="s">
-        <v>83</v>
-      </c>
-      <c r="G61" s="95"/>
-      <c r="H61" s="144">
+      <c r="E61" s="141" t="s">
+        <v>61</v>
+      </c>
+      <c r="F61" s="142">
+        <v>1.5</v>
+      </c>
+      <c r="G61" s="94"/>
+      <c r="H61" s="143">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="I61" s="95"/>
-      <c r="J61" s="5"/>
+      <c r="I61" s="94"/>
+      <c r="J61" s="82" t="s">
+        <v>67</v>
+      </c>
       <c r="K61" s="5"/>
       <c r="L61" s="5"/>
-      <c r="M61" s="146"/>
-      <c r="N61" s="146"/>
-      <c r="O61" s="146"/>
-      <c r="P61" s="146"/>
-      <c r="Q61" s="146">
+      <c r="M61" s="145"/>
+      <c r="N61" s="145"/>
+      <c r="O61" s="145"/>
+      <c r="P61" s="145"/>
+      <c r="Q61" s="145">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4466,30 +4704,30 @@
     </row>
     <row r="62" ht="15.0" customHeight="1">
       <c r="A62" s="68"/>
-      <c r="B62" s="147" t="s">
+      <c r="B62" s="148" t="s">
         <v>71</v>
       </c>
-      <c r="C62" s="148"/>
-      <c r="D62" s="149"/>
-      <c r="E62" s="150"/>
-      <c r="F62" s="151"/>
-      <c r="G62" s="152">
+      <c r="C62" s="149"/>
+      <c r="D62" s="150"/>
+      <c r="E62" s="151"/>
+      <c r="F62" s="152"/>
+      <c r="G62" s="153">
         <f>SUM(F63:F64)</f>
-        <v>0</v>
-      </c>
-      <c r="H62" s="151"/>
-      <c r="I62" s="153">
+        <v>4</v>
+      </c>
+      <c r="H62" s="152"/>
+      <c r="I62" s="154">
         <f>SUM(H63:H64)</f>
         <v>0</v>
       </c>
       <c r="J62" s="5"/>
       <c r="K62" s="5"/>
       <c r="L62" s="5"/>
-      <c r="M62" s="154"/>
-      <c r="N62" s="154"/>
-      <c r="O62" s="154"/>
-      <c r="P62" s="154"/>
-      <c r="Q62" s="154">
+      <c r="M62" s="155"/>
+      <c r="N62" s="155"/>
+      <c r="O62" s="155"/>
+      <c r="P62" s="155"/>
+      <c r="Q62" s="155">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4510,32 +4748,36 @@
       <c r="AF62" s="5"/>
     </row>
     <row r="63" ht="15.0" customHeight="1">
-      <c r="A63" s="128"/>
-      <c r="B63" s="129"/>
+      <c r="A63" s="125"/>
+      <c r="B63" s="126"/>
       <c r="C63" s="60" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D63" s="61" t="s">
-        <v>105</v>
-      </c>
-      <c r="E63" s="62"/>
-      <c r="F63" s="155" t="s">
-        <v>83</v>
-      </c>
-      <c r="G63" s="132"/>
-      <c r="H63" s="156">
+        <v>107</v>
+      </c>
+      <c r="E63" s="156" t="s">
+        <v>108</v>
+      </c>
+      <c r="F63" s="157">
+        <v>2.0</v>
+      </c>
+      <c r="G63" s="129"/>
+      <c r="H63" s="158">
         <f t="shared" ref="H63:H65" si="11">SUM(M63:P63)</f>
         <v>0</v>
       </c>
-      <c r="I63" s="133"/>
-      <c r="J63" s="5"/>
+      <c r="I63" s="130"/>
+      <c r="J63" s="82" t="s">
+        <v>67</v>
+      </c>
       <c r="K63" s="5"/>
       <c r="L63" s="5"/>
-      <c r="M63" s="134"/>
-      <c r="N63" s="134"/>
-      <c r="O63" s="135"/>
-      <c r="P63" s="135"/>
-      <c r="Q63" s="135">
+      <c r="M63" s="159"/>
+      <c r="N63" s="159"/>
+      <c r="O63" s="132"/>
+      <c r="P63" s="132"/>
+      <c r="Q63" s="132">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4556,32 +4798,36 @@
       <c r="AF63" s="5"/>
     </row>
     <row r="64" ht="15.0" customHeight="1">
-      <c r="A64" s="157"/>
-      <c r="B64" s="90"/>
-      <c r="C64" s="141" t="s">
+      <c r="A64" s="160"/>
+      <c r="B64" s="89"/>
+      <c r="C64" s="147" t="s">
         <v>96</v>
       </c>
-      <c r="D64" s="92" t="s">
-        <v>75</v>
-      </c>
-      <c r="E64" s="158"/>
-      <c r="F64" s="143" t="s">
-        <v>83</v>
-      </c>
-      <c r="G64" s="95"/>
-      <c r="H64" s="144">
+      <c r="D64" s="91" t="s">
+        <v>74</v>
+      </c>
+      <c r="E64" s="161" t="s">
+        <v>109</v>
+      </c>
+      <c r="F64" s="142">
+        <v>2.0</v>
+      </c>
+      <c r="G64" s="94"/>
+      <c r="H64" s="143">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="I64" s="95"/>
-      <c r="J64" s="5"/>
+      <c r="I64" s="94"/>
+      <c r="J64" s="82" t="s">
+        <v>67</v>
+      </c>
       <c r="K64" s="5"/>
       <c r="L64" s="5"/>
-      <c r="M64" s="145"/>
-      <c r="N64" s="146"/>
-      <c r="O64" s="146"/>
-      <c r="P64" s="145"/>
-      <c r="Q64" s="146">
+      <c r="M64" s="144"/>
+      <c r="N64" s="145"/>
+      <c r="O64" s="145"/>
+      <c r="P64" s="144"/>
+      <c r="Q64" s="145">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4602,73 +4848,73 @@
       <c r="AF64" s="5"/>
     </row>
     <row r="65" ht="12.75" customHeight="1">
-      <c r="A65" s="159" t="s">
+      <c r="A65" s="162" t="s">
         <v>6</v>
       </c>
-      <c r="B65" s="159"/>
-      <c r="C65" s="160"/>
-      <c r="D65" s="160"/>
-      <c r="E65" s="161"/>
-      <c r="F65" s="162">
+      <c r="B65" s="162"/>
+      <c r="C65" s="163"/>
+      <c r="D65" s="163"/>
+      <c r="E65" s="164"/>
+      <c r="F65" s="165">
         <f t="shared" ref="F65:G65" si="12">SUM(F5:F64)</f>
-        <v>136.5</v>
-      </c>
-      <c r="G65" s="163">
+        <v>172</v>
+      </c>
+      <c r="G65" s="166">
         <f t="shared" si="12"/>
-        <v>136.5</v>
-      </c>
-      <c r="H65" s="164">
+        <v>172</v>
+      </c>
+      <c r="H65" s="167">
         <f t="shared" si="11"/>
-        <v>44.4</v>
-      </c>
-      <c r="I65" s="163">
+        <v>68</v>
+      </c>
+      <c r="I65" s="166">
         <f>SUM(I5:I64)</f>
-        <v>44.4</v>
-      </c>
-      <c r="J65" s="165"/>
-      <c r="K65" s="165"/>
-      <c r="L65" s="165"/>
-      <c r="M65" s="164">
+        <v>68</v>
+      </c>
+      <c r="J65" s="168"/>
+      <c r="K65" s="168"/>
+      <c r="L65" s="168"/>
+      <c r="M65" s="167">
         <f t="shared" ref="M65:P65" si="13">SUM(M5:M64)</f>
-        <v>16.6</v>
-      </c>
-      <c r="N65" s="164">
+        <v>24.2</v>
+      </c>
+      <c r="N65" s="167">
         <f t="shared" si="13"/>
-        <v>10</v>
-      </c>
-      <c r="O65" s="164">
+        <v>16.45</v>
+      </c>
+      <c r="O65" s="167">
         <f t="shared" si="13"/>
-        <v>11.9</v>
-      </c>
-      <c r="P65" s="164">
+        <v>18.65</v>
+      </c>
+      <c r="P65" s="167">
         <f t="shared" si="13"/>
-        <v>5.9</v>
-      </c>
-      <c r="Q65" s="164">
+        <v>8.7</v>
+      </c>
+      <c r="Q65" s="167">
         <f t="shared" si="1"/>
-        <v>44.4</v>
-      </c>
-      <c r="R65" s="165"/>
-      <c r="S65" s="165"/>
-      <c r="T65" s="165"/>
-      <c r="U65" s="165"/>
-      <c r="V65" s="165"/>
-      <c r="W65" s="165"/>
-      <c r="X65" s="165"/>
-      <c r="Y65" s="165"/>
-      <c r="Z65" s="165"/>
-      <c r="AA65" s="165"/>
-      <c r="AB65" s="165"/>
-      <c r="AC65" s="165"/>
-      <c r="AD65" s="165"/>
-      <c r="AE65" s="165"/>
-      <c r="AF65" s="165"/>
+        <v>68</v>
+      </c>
+      <c r="R65" s="168"/>
+      <c r="S65" s="168"/>
+      <c r="T65" s="168"/>
+      <c r="U65" s="168"/>
+      <c r="V65" s="168"/>
+      <c r="W65" s="168"/>
+      <c r="X65" s="168"/>
+      <c r="Y65" s="168"/>
+      <c r="Z65" s="168"/>
+      <c r="AA65" s="168"/>
+      <c r="AB65" s="168"/>
+      <c r="AC65" s="168"/>
+      <c r="AD65" s="168"/>
+      <c r="AE65" s="168"/>
+      <c r="AF65" s="168"/>
     </row>
     <row r="66" ht="12.75" customHeight="1">
       <c r="A66" s="9"/>
       <c r="B66" s="9"/>
       <c r="C66" s="9"/>
-      <c r="D66" s="166"/>
+      <c r="D66" s="169"/>
       <c r="E66" s="9"/>
       <c r="F66" s="9"/>
       <c r="G66" s="9"/>
@@ -4702,7 +4948,7 @@
       <c r="A67" s="9"/>
       <c r="B67" s="9"/>
       <c r="C67" s="9"/>
-      <c r="D67" s="166"/>
+      <c r="D67" s="169"/>
       <c r="E67" s="9"/>
       <c r="F67" s="9"/>
       <c r="G67" s="9"/>
@@ -4736,7 +4982,7 @@
       <c r="A68" s="9"/>
       <c r="B68" s="9"/>
       <c r="C68" s="9"/>
-      <c r="D68" s="166"/>
+      <c r="D68" s="169"/>
       <c r="E68" s="9"/>
       <c r="F68" s="9"/>
       <c r="G68" s="9"/>

</xml_diff>

<commit_message>
Added relevant documentation for Iteration #4
</commit_message>
<xml_diff>
--- a/documentation/CS451R.Group14.EffortEstimate.xlsx
+++ b/documentation/CS451R.Group14.EffortEstimate.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="133">
   <si>
     <t>Note: Beyond Iteration 2, nothing is changed.</t>
   </si>
@@ -601,6 +601,85 @@
       <t>, Zach Zoltek</t>
     </r>
   </si>
+  <si>
+    <t>Iteration 5:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Samuel Lim, </t>
+    </r>
+    <r>
+      <rPr/>
+      <t>Alivia Dutcher</t>
+    </r>
+  </si>
+  <si>
+    <t>Finalise schedule UI actions</t>
+  </si>
+  <si>
+    <t>Design final conflict representation in UI</t>
+  </si>
+  <si>
+    <t>Develop generic constraints for scheduling engine</t>
+  </si>
+  <si>
+    <r>
+      <t>Alivia Dutcher,</t>
+    </r>
+    <r>
+      <rPr/>
+      <t xml:space="preserve"> Samuel Lim</t>
+    </r>
+  </si>
+  <si>
+    <t>Finalise database profile saving</t>
+  </si>
+  <si>
+    <t>Implement client live-loading</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Zach Zoltek, </t>
+    </r>
+    <r>
+      <rPr/>
+      <t>Samuel Lim</t>
+    </r>
+  </si>
+  <si>
+    <t>Acceptance, Performance, Regression Tests</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t>Zach Zoltek</t>
+    </r>
+    <r>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <t>Samuel Lim, Alivia Dutcher</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t>Alivia Dutcher</t>
+    </r>
+    <r>
+      <t>, Zach Zoltek</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -655,12 +734,12 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="10.0"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <sz val="12.0"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10.0"/>
-      <name val="Arial"/>
     </font>
     <font>
       <b/>
@@ -857,7 +936,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="202">
+  <cellXfs count="222">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1263,8 +1342,8 @@
     <xf borderId="10" fillId="5" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="10" fillId="5" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="11" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -1280,9 +1359,6 @@
     </xf>
     <xf borderId="4" fillId="5" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="5" fontId="9" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="4" fillId="5" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
@@ -1329,89 +1405,47 @@
     <xf borderId="14" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
     <xf borderId="5" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="5" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="13" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="13" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="13" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="13" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="13" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="13" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="13" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="13" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="9" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="13" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="13" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="13" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="13" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="9" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="13" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="13" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="13" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="11" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="11" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="10" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="11" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="5" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -1419,10 +1453,7 @@
     <xf borderId="1" fillId="3" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="13" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1434,11 +1465,122 @@
     <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="14" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="14" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="5" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="13" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="13" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="3" fillId="5" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="5" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="5" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="13" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="10" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="11" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="10" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="12" fillId="5" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="11" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="11" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="5" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="5" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="5" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="7" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="7" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="9" fillId="4" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="10" fillId="5" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="14" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="9" fillId="6" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
@@ -1460,9 +1602,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4439,7 +4578,7 @@
         <v>0.9</v>
       </c>
       <c r="I53" s="78"/>
-      <c r="J53" s="135" t="s">
+      <c r="J53" s="81" t="s">
         <v>57</v>
       </c>
       <c r="K53" s="5"/>
@@ -4453,7 +4592,9 @@
       <c r="O53" s="100">
         <v>0.3</v>
       </c>
-      <c r="P53" s="101"/>
+      <c r="P53" s="135">
+        <v>0.0</v>
+      </c>
       <c r="Q53" s="101">
         <f t="shared" si="1"/>
         <v>0.9</v>
@@ -4495,22 +4636,22 @@
         <v>0</v>
       </c>
       <c r="I54" s="78"/>
-      <c r="J54" s="135" t="s">
+      <c r="J54" s="81" t="s">
         <v>54</v>
       </c>
       <c r="K54" s="5"/>
       <c r="L54" s="5"/>
-      <c r="M54" s="100" t="s">
-        <v>82</v>
-      </c>
-      <c r="N54" s="100" t="s">
-        <v>82</v>
-      </c>
-      <c r="O54" s="100" t="s">
-        <v>82</v>
-      </c>
-      <c r="P54" s="100" t="s">
-        <v>82</v>
+      <c r="M54" s="135">
+        <v>0.0</v>
+      </c>
+      <c r="N54" s="135">
+        <v>0.0</v>
+      </c>
+      <c r="O54" s="135">
+        <v>0.0</v>
+      </c>
+      <c r="P54" s="135">
+        <v>0.0</v>
       </c>
       <c r="Q54" s="101">
         <f t="shared" si="1"/>
@@ -4555,7 +4696,7 @@
         <v>1.5</v>
       </c>
       <c r="I55" s="92"/>
-      <c r="J55" s="135" t="s">
+      <c r="J55" s="81" t="s">
         <v>81</v>
       </c>
       <c r="K55" s="5"/>
@@ -4563,12 +4704,12 @@
       <c r="M55" s="141">
         <v>0.5</v>
       </c>
-      <c r="N55" s="142">
+      <c r="N55" s="141">
         <v>1.0</v>
       </c>
-      <c r="O55" s="143"/>
-      <c r="P55" s="143"/>
-      <c r="Q55" s="143">
+      <c r="O55" s="142"/>
+      <c r="P55" s="142"/>
+      <c r="Q55" s="142">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
@@ -4708,12 +4849,12 @@
         <v>0</v>
       </c>
       <c r="I58" s="78"/>
-      <c r="J58" s="135" t="s">
+      <c r="J58" s="81" t="s">
         <v>81</v>
       </c>
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
-      <c r="M58" s="101"/>
+      <c r="M58" s="135"/>
       <c r="N58" s="101"/>
       <c r="O58" s="101"/>
       <c r="P58" s="100"/>
@@ -4840,7 +4981,7 @@
     <row r="61" ht="15.0" customHeight="1">
       <c r="A61" s="67"/>
       <c r="B61" s="87"/>
-      <c r="C61" s="144" t="s">
+      <c r="C61" s="143" t="s">
         <v>69</v>
       </c>
       <c r="D61" s="89" t="s">
@@ -4858,16 +4999,16 @@
         <v>0</v>
       </c>
       <c r="I61" s="92"/>
-      <c r="J61" s="135" t="s">
+      <c r="J61" s="81" t="s">
         <v>54</v>
       </c>
       <c r="K61" s="5"/>
       <c r="L61" s="5"/>
-      <c r="M61" s="143"/>
-      <c r="N61" s="143"/>
-      <c r="O61" s="143"/>
-      <c r="P61" s="143"/>
-      <c r="Q61" s="143">
+      <c r="M61" s="142"/>
+      <c r="N61" s="142"/>
+      <c r="O61" s="142"/>
+      <c r="P61" s="142"/>
+      <c r="Q61" s="142">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4889,30 +5030,30 @@
     </row>
     <row r="62" ht="15.0" customHeight="1">
       <c r="A62" s="67"/>
-      <c r="B62" s="145" t="s">
+      <c r="B62" s="144" t="s">
         <v>71</v>
       </c>
-      <c r="C62" s="146"/>
-      <c r="D62" s="147"/>
-      <c r="E62" s="148"/>
-      <c r="F62" s="149"/>
-      <c r="G62" s="150">
+      <c r="C62" s="145"/>
+      <c r="D62" s="146"/>
+      <c r="E62" s="147"/>
+      <c r="F62" s="148"/>
+      <c r="G62" s="149">
         <f>SUM(F63:F64)</f>
         <v>4</v>
       </c>
-      <c r="H62" s="149"/>
-      <c r="I62" s="151">
+      <c r="H62" s="148"/>
+      <c r="I62" s="150">
         <f>SUM(H63:H64)</f>
         <v>0</v>
       </c>
       <c r="J62" s="5"/>
       <c r="K62" s="5"/>
       <c r="L62" s="5"/>
-      <c r="M62" s="152"/>
-      <c r="N62" s="152"/>
-      <c r="O62" s="152"/>
-      <c r="P62" s="152"/>
-      <c r="Q62" s="152">
+      <c r="M62" s="151"/>
+      <c r="N62" s="151"/>
+      <c r="O62" s="151"/>
+      <c r="P62" s="151"/>
+      <c r="Q62" s="151">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4941,19 +5082,19 @@
       <c r="D63" s="60" t="s">
         <v>107</v>
       </c>
-      <c r="E63" s="153" t="s">
+      <c r="E63" s="152" t="s">
         <v>108</v>
       </c>
-      <c r="F63" s="154">
+      <c r="F63" s="153">
         <v>2.0</v>
       </c>
       <c r="G63" s="127"/>
-      <c r="H63" s="155">
+      <c r="H63" s="154">
         <f t="shared" ref="H63:H64" si="11">SUM(M63:P63)</f>
         <v>0</v>
       </c>
       <c r="I63" s="128"/>
-      <c r="J63" s="135" t="s">
+      <c r="J63" s="81" t="s">
         <v>54</v>
       </c>
       <c r="K63" s="5"/>
@@ -4983,36 +5124,36 @@
       <c r="AF63" s="5"/>
     </row>
     <row r="64" ht="15.0" customHeight="1">
-      <c r="A64" s="156"/>
-      <c r="B64" s="157"/>
-      <c r="C64" s="158" t="s">
+      <c r="A64" s="155"/>
+      <c r="B64" s="87"/>
+      <c r="C64" s="143" t="s">
         <v>96</v>
       </c>
       <c r="D64" s="89" t="s">
         <v>74</v>
       </c>
-      <c r="E64" s="159" t="s">
+      <c r="E64" s="156" t="s">
         <v>109</v>
       </c>
-      <c r="F64" s="160">
+      <c r="F64" s="139">
         <v>2.0</v>
       </c>
-      <c r="G64" s="161"/>
+      <c r="G64" s="92"/>
       <c r="H64" s="140">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="I64" s="161"/>
-      <c r="J64" s="135" t="s">
+      <c r="I64" s="92"/>
+      <c r="J64" s="81" t="s">
         <v>76</v>
       </c>
       <c r="K64" s="5"/>
       <c r="L64" s="5"/>
-      <c r="M64" s="142"/>
-      <c r="N64" s="143"/>
-      <c r="O64" s="143"/>
-      <c r="P64" s="142"/>
-      <c r="Q64" s="143">
+      <c r="M64" s="141"/>
+      <c r="N64" s="142"/>
+      <c r="O64" s="142"/>
+      <c r="P64" s="141"/>
+      <c r="Q64" s="142">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5033,15 +5174,15 @@
       <c r="AF64" s="5"/>
     </row>
     <row r="65" ht="18.75" customHeight="1">
-      <c r="A65" s="162" t="s">
+      <c r="A65" s="157" t="s">
         <v>110</v>
       </c>
-      <c r="B65" s="163" t="s">
+      <c r="B65" s="158" t="s">
         <v>79</v>
       </c>
       <c r="C65" s="69"/>
-      <c r="D65" s="164"/>
-      <c r="E65" s="165"/>
+      <c r="D65" s="70"/>
+      <c r="E65" s="104"/>
       <c r="F65" s="69"/>
       <c r="G65" s="105">
         <f>SUM(F66:F68)</f>
@@ -5050,62 +5191,70 @@
       <c r="H65" s="69"/>
       <c r="I65" s="106">
         <f>SUM(H66:H68)</f>
-        <v>0</v>
-      </c>
-      <c r="M65" s="165"/>
+        <v>8</v>
+      </c>
+      <c r="M65" s="104"/>
       <c r="N65" s="69"/>
-      <c r="O65" s="165"/>
+      <c r="O65" s="104"/>
       <c r="P65" s="69"/>
-      <c r="Q65" s="164"/>
-      <c r="R65" s="166"/>
-      <c r="S65" s="166"/>
-      <c r="T65" s="166"/>
-      <c r="U65" s="166"/>
-      <c r="V65" s="166"/>
-      <c r="W65" s="166"/>
-      <c r="X65" s="166"/>
-      <c r="Y65" s="166"/>
-      <c r="Z65" s="166"/>
-      <c r="AA65" s="166"/>
-      <c r="AB65" s="166"/>
-      <c r="AC65" s="166"/>
-      <c r="AD65" s="166"/>
-      <c r="AE65" s="166"/>
-      <c r="AF65" s="166"/>
+      <c r="Q65" s="70"/>
+      <c r="R65" s="159"/>
+      <c r="S65" s="159"/>
+      <c r="T65" s="159"/>
+      <c r="U65" s="159"/>
+      <c r="V65" s="159"/>
+      <c r="W65" s="159"/>
+      <c r="X65" s="159"/>
+      <c r="Y65" s="159"/>
+      <c r="Z65" s="159"/>
+      <c r="AA65" s="159"/>
+      <c r="AB65" s="159"/>
+      <c r="AC65" s="159"/>
+      <c r="AD65" s="159"/>
+      <c r="AE65" s="159"/>
+      <c r="AF65" s="159"/>
     </row>
     <row r="66" ht="16.5" customHeight="1">
-      <c r="A66" s="167"/>
-      <c r="B66" s="167"/>
-      <c r="C66" s="167" t="s">
+      <c r="A66" s="160"/>
+      <c r="B66" s="160"/>
+      <c r="C66" s="160" t="s">
         <v>80</v>
       </c>
-      <c r="D66" s="168" t="s">
+      <c r="D66" s="161" t="s">
         <v>20</v>
       </c>
-      <c r="E66" s="169" t="s">
+      <c r="E66" s="162" t="s">
         <v>21</v>
       </c>
-      <c r="F66" s="169">
+      <c r="F66" s="162">
         <v>2.0</v>
       </c>
-      <c r="G66" s="167"/>
+      <c r="G66" s="160"/>
       <c r="H66" s="45">
         <f t="shared" ref="H66:H68" si="12">SUM(M66:P66)</f>
-        <v>0</v>
-      </c>
-      <c r="I66" s="167"/>
-      <c r="J66" s="135" t="s">
-        <v>67</v>
+        <v>3</v>
+      </c>
+      <c r="I66" s="160"/>
+      <c r="J66" s="163" t="s">
+        <v>81</v>
       </c>
       <c r="K66" s="9"/>
       <c r="L66" s="9"/>
-      <c r="M66" s="170"/>
-      <c r="N66" s="170"/>
-      <c r="O66" s="170"/>
-      <c r="P66" s="170"/>
-      <c r="Q66" s="171">
+      <c r="M66" s="164">
+        <v>3.0</v>
+      </c>
+      <c r="N66" s="164" t="s">
+        <v>82</v>
+      </c>
+      <c r="O66" s="164" t="s">
+        <v>82</v>
+      </c>
+      <c r="P66" s="164" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q66" s="165">
         <f t="shared" ref="Q66:Q68" si="13">SUM(M66:P66)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R66" s="9"/>
       <c r="S66" s="9"/>
@@ -5124,38 +5273,46 @@
       <c r="AF66" s="9"/>
     </row>
     <row r="67" ht="16.5" customHeight="1">
-      <c r="A67" s="172"/>
-      <c r="B67" s="172"/>
-      <c r="C67" s="167" t="s">
+      <c r="A67" s="103"/>
+      <c r="B67" s="103"/>
+      <c r="C67" s="160" t="s">
         <v>83</v>
       </c>
-      <c r="D67" s="168" t="s">
+      <c r="D67" s="161" t="s">
         <v>20</v>
       </c>
-      <c r="E67" s="173" t="s">
+      <c r="E67" s="166" t="s">
         <v>111</v>
       </c>
-      <c r="F67" s="169">
+      <c r="F67" s="162">
         <v>4.0</v>
       </c>
-      <c r="G67" s="172"/>
+      <c r="G67" s="103"/>
       <c r="H67" s="45">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="I67" s="172"/>
-      <c r="J67" s="135" t="s">
-        <v>54</v>
+        <v>3.5</v>
+      </c>
+      <c r="I67" s="103"/>
+      <c r="J67" s="163" t="s">
+        <v>57</v>
       </c>
       <c r="K67" s="9"/>
       <c r="L67" s="9"/>
-      <c r="M67" s="170"/>
-      <c r="N67" s="174"/>
-      <c r="O67" s="174"/>
-      <c r="P67" s="174"/>
-      <c r="Q67" s="171">
+      <c r="M67" s="164">
+        <v>1.0</v>
+      </c>
+      <c r="N67" s="164">
+        <v>1.0</v>
+      </c>
+      <c r="O67" s="164">
+        <v>1.0</v>
+      </c>
+      <c r="P67" s="164">
+        <v>0.5</v>
+      </c>
+      <c r="Q67" s="165">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="R67" s="9"/>
       <c r="S67" s="9"/>
@@ -5174,40 +5331,48 @@
       <c r="AF67" s="9"/>
     </row>
     <row r="68" ht="16.5" customHeight="1">
-      <c r="A68" s="172"/>
-      <c r="B68" s="172"/>
-      <c r="C68" s="175" t="s">
+      <c r="A68" s="103"/>
+      <c r="B68" s="103"/>
+      <c r="C68" s="167" t="s">
         <v>88</v>
       </c>
-      <c r="D68" s="168" t="s">
+      <c r="D68" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="E68" s="176" t="s">
+      <c r="E68" s="168" t="s">
         <v>61</v>
       </c>
-      <c r="F68" s="169">
+      <c r="F68" s="162">
         <v>4.0</v>
       </c>
-      <c r="G68" s="172"/>
+      <c r="G68" s="103"/>
       <c r="H68" s="45">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="I68" s="172"/>
-      <c r="J68" s="135" t="s">
-        <v>54</v>
+        <v>1.5</v>
+      </c>
+      <c r="I68" s="103"/>
+      <c r="J68" s="163" t="s">
+        <v>57</v>
       </c>
       <c r="K68" s="9"/>
       <c r="L68" s="9"/>
-      <c r="M68" s="170"/>
-      <c r="N68" s="174"/>
-      <c r="O68" s="174"/>
-      <c r="P68" s="174"/>
-      <c r="Q68" s="171">
+      <c r="M68" s="164" t="s">
+        <v>82</v>
+      </c>
+      <c r="N68" s="164">
+        <v>1.5</v>
+      </c>
+      <c r="O68" s="164" t="s">
+        <v>82</v>
+      </c>
+      <c r="P68" s="164" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q68" s="165">
         <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="R68" s="135" t="s">
+        <v>1.5</v>
+      </c>
+      <c r="R68" s="81" t="s">
         <v>112</v>
       </c>
       <c r="S68" s="9"/>
@@ -5226,13 +5391,13 @@
       <c r="AF68" s="9"/>
     </row>
     <row r="69">
-      <c r="A69" s="172"/>
-      <c r="B69" s="163" t="s">
+      <c r="A69" s="103"/>
+      <c r="B69" s="158" t="s">
         <v>50</v>
       </c>
       <c r="C69" s="69"/>
-      <c r="D69" s="164"/>
-      <c r="E69" s="165"/>
+      <c r="D69" s="70"/>
+      <c r="E69" s="104"/>
       <c r="F69" s="69"/>
       <c r="G69" s="105">
         <f>SUM(F70:F77)</f>
@@ -5241,16 +5406,16 @@
       <c r="H69" s="69"/>
       <c r="I69" s="106">
         <f>SUM(H70:H77)</f>
-        <v>0</v>
+        <v>15.3</v>
       </c>
       <c r="J69" s="5"/>
       <c r="K69" s="5"/>
       <c r="L69" s="5"/>
-      <c r="M69" s="165"/>
+      <c r="M69" s="104"/>
       <c r="N69" s="69"/>
-      <c r="O69" s="165"/>
+      <c r="O69" s="104"/>
       <c r="P69" s="69"/>
-      <c r="Q69" s="164"/>
+      <c r="Q69" s="70"/>
       <c r="R69" s="5"/>
       <c r="S69" s="5"/>
       <c r="T69" s="5"/>
@@ -5268,38 +5433,46 @@
       <c r="AF69" s="5"/>
     </row>
     <row r="70">
-      <c r="A70" s="162"/>
-      <c r="B70" s="172"/>
-      <c r="C70" s="177" t="s">
+      <c r="A70" s="157"/>
+      <c r="B70" s="103"/>
+      <c r="C70" s="40" t="s">
         <v>89</v>
       </c>
       <c r="D70" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="E70" s="178" t="s">
+      <c r="E70" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="F70" s="179">
+      <c r="F70" s="43">
         <v>2.0</v>
       </c>
-      <c r="G70" s="172"/>
+      <c r="G70" s="103"/>
       <c r="H70" s="45">
         <f t="shared" ref="H70:H75" si="14">SUM(M70:P70)</f>
-        <v>0</v>
-      </c>
-      <c r="I70" s="172"/>
-      <c r="J70" s="135" t="s">
-        <v>67</v>
+        <v>4</v>
+      </c>
+      <c r="I70" s="103"/>
+      <c r="J70" s="163" t="s">
+        <v>57</v>
       </c>
       <c r="K70" s="5"/>
       <c r="L70" s="5"/>
-      <c r="M70" s="170"/>
-      <c r="N70" s="174"/>
-      <c r="O70" s="174"/>
-      <c r="P70" s="174"/>
-      <c r="Q70" s="171">
-        <f t="shared" ref="Q70:Q75" si="15">SUM(M70:P70)</f>
-        <v>0</v>
+      <c r="M70" s="164">
+        <v>1.5</v>
+      </c>
+      <c r="N70" s="164">
+        <v>1.5</v>
+      </c>
+      <c r="O70" s="164">
+        <v>1.0</v>
+      </c>
+      <c r="P70" s="164" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q70" s="165">
+        <f t="shared" ref="Q70:Q77" si="15">SUM(M70:P70)</f>
+        <v>4</v>
       </c>
       <c r="R70" s="5"/>
       <c r="S70" s="5"/>
@@ -5318,9 +5491,9 @@
       <c r="AF70" s="5"/>
     </row>
     <row r="71">
-      <c r="A71" s="162"/>
-      <c r="B71" s="172"/>
-      <c r="C71" s="180" t="s">
+      <c r="A71" s="157"/>
+      <c r="B71" s="103"/>
+      <c r="C71" s="112" t="s">
         <v>102</v>
       </c>
       <c r="D71" s="41" t="s">
@@ -5329,29 +5502,37 @@
       <c r="E71" s="42" t="s">
         <v>113</v>
       </c>
-      <c r="F71" s="179">
+      <c r="F71" s="43">
         <v>6.0</v>
       </c>
-      <c r="G71" s="172"/>
+      <c r="G71" s="103"/>
       <c r="H71" s="45">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="I71" s="172"/>
-      <c r="J71" s="135" t="s">
-        <v>67</v>
+        <v>3</v>
+      </c>
+      <c r="I71" s="103"/>
+      <c r="J71" s="163" t="s">
+        <v>54</v>
       </c>
       <c r="K71" s="5"/>
       <c r="L71" s="5"/>
-      <c r="M71" s="170"/>
-      <c r="N71" s="174"/>
-      <c r="O71" s="174"/>
-      <c r="P71" s="174"/>
-      <c r="Q71" s="171">
+      <c r="M71" s="164">
+        <v>2.0</v>
+      </c>
+      <c r="N71" s="164">
+        <v>1.0</v>
+      </c>
+      <c r="O71" s="164" t="s">
+        <v>82</v>
+      </c>
+      <c r="P71" s="164" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q71" s="165">
         <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="R71" s="135" t="s">
+        <v>3</v>
+      </c>
+      <c r="R71" s="81" t="s">
         <v>112</v>
       </c>
       <c r="S71" s="5"/>
@@ -5370,40 +5551,48 @@
       <c r="AF71" s="5"/>
     </row>
     <row r="72">
-      <c r="A72" s="162"/>
-      <c r="B72" s="162"/>
-      <c r="C72" s="180" t="s">
+      <c r="A72" s="157"/>
+      <c r="B72" s="157"/>
+      <c r="C72" s="112" t="s">
         <v>104</v>
       </c>
       <c r="D72" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="E72" s="178" t="s">
+      <c r="E72" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="F72" s="179">
+      <c r="F72" s="43">
         <v>6.0</v>
       </c>
-      <c r="G72" s="172"/>
+      <c r="G72" s="103"/>
       <c r="H72" s="45">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="I72" s="172"/>
-      <c r="J72" s="135" t="s">
-        <v>67</v>
+      <c r="I72" s="103"/>
+      <c r="J72" s="163" t="s">
+        <v>54</v>
       </c>
       <c r="K72" s="5"/>
       <c r="L72" s="5"/>
-      <c r="M72" s="170"/>
-      <c r="N72" s="174"/>
-      <c r="O72" s="174"/>
-      <c r="P72" s="174"/>
-      <c r="Q72" s="171">
+      <c r="M72" s="164" t="s">
+        <v>82</v>
+      </c>
+      <c r="N72" s="164" t="s">
+        <v>82</v>
+      </c>
+      <c r="O72" s="164" t="s">
+        <v>82</v>
+      </c>
+      <c r="P72" s="164" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q72" s="165">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="R72" s="135" t="s">
+      <c r="R72" s="81" t="s">
         <v>112</v>
       </c>
       <c r="S72" s="5"/>
@@ -5422,40 +5611,48 @@
       <c r="AF72" s="5"/>
     </row>
     <row r="73">
-      <c r="A73" s="162"/>
-      <c r="B73" s="162"/>
-      <c r="C73" s="180" t="s">
+      <c r="A73" s="157"/>
+      <c r="B73" s="157"/>
+      <c r="C73" s="112" t="s">
         <v>105</v>
       </c>
       <c r="D73" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="E73" s="178" t="s">
+      <c r="E73" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="F73" s="179">
+      <c r="F73" s="43">
         <v>4.0</v>
       </c>
-      <c r="G73" s="172"/>
+      <c r="G73" s="103"/>
       <c r="H73" s="45">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="I73" s="172"/>
-      <c r="J73" s="135" t="s">
-        <v>67</v>
+        <v>1.6</v>
+      </c>
+      <c r="I73" s="169"/>
+      <c r="J73" s="163" t="s">
+        <v>81</v>
       </c>
       <c r="K73" s="5"/>
       <c r="L73" s="5"/>
-      <c r="M73" s="170"/>
-      <c r="N73" s="174"/>
-      <c r="O73" s="174"/>
-      <c r="P73" s="174"/>
-      <c r="Q73" s="171">
+      <c r="M73" s="164">
+        <v>0.6</v>
+      </c>
+      <c r="N73" s="164">
+        <v>1.0</v>
+      </c>
+      <c r="O73" s="164" t="s">
+        <v>82</v>
+      </c>
+      <c r="P73" s="164" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q73" s="165">
         <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="R73" s="135" t="s">
+        <v>1.6</v>
+      </c>
+      <c r="R73" s="81" t="s">
         <v>112</v>
       </c>
       <c r="S73" s="5"/>
@@ -5474,38 +5671,46 @@
       <c r="AF73" s="5"/>
     </row>
     <row r="74">
-      <c r="A74" s="172"/>
-      <c r="B74" s="162"/>
-      <c r="C74" s="181" t="s">
+      <c r="A74" s="103"/>
+      <c r="B74" s="157"/>
+      <c r="C74" s="50" t="s">
         <v>69</v>
       </c>
       <c r="D74" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="E74" s="182" t="s">
+      <c r="E74" s="52" t="s">
         <v>61</v>
       </c>
-      <c r="F74" s="183">
+      <c r="F74" s="115">
         <v>1.5</v>
       </c>
-      <c r="G74" s="172"/>
+      <c r="G74" s="103"/>
       <c r="H74" s="45">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="I74" s="172"/>
-      <c r="J74" s="135" t="s">
-        <v>67</v>
+        <v>0.2</v>
+      </c>
+      <c r="I74" s="169"/>
+      <c r="J74" s="163" t="s">
+        <v>57</v>
       </c>
       <c r="K74" s="5"/>
       <c r="L74" s="5"/>
-      <c r="M74" s="170"/>
-      <c r="N74" s="174"/>
-      <c r="O74" s="174"/>
-      <c r="P74" s="174"/>
-      <c r="Q74" s="171">
+      <c r="M74" s="164">
+        <v>0.2</v>
+      </c>
+      <c r="N74" s="164" t="s">
+        <v>82</v>
+      </c>
+      <c r="O74" s="164" t="s">
+        <v>82</v>
+      </c>
+      <c r="P74" s="164" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q74" s="165">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="R74" s="5"/>
       <c r="S74" s="5"/>
@@ -5525,37 +5730,45 @@
     </row>
     <row r="75">
       <c r="A75" s="103"/>
-      <c r="B75" s="162"/>
-      <c r="C75" s="184" t="s">
+      <c r="B75" s="157"/>
+      <c r="C75" s="114" t="s">
         <v>114</v>
       </c>
-      <c r="D75" s="185" t="s">
+      <c r="D75" s="170" t="s">
         <v>52</v>
       </c>
-      <c r="E75" s="182" t="s">
+      <c r="E75" s="52" t="s">
         <v>61</v>
       </c>
-      <c r="F75" s="183">
+      <c r="F75" s="115">
         <v>3.5</v>
       </c>
       <c r="G75" s="103"/>
       <c r="H75" s="45">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="I75" s="103"/>
-      <c r="J75" s="135" t="s">
-        <v>67</v>
+        <v>4</v>
+      </c>
+      <c r="I75" s="169"/>
+      <c r="J75" s="163" t="s">
+        <v>81</v>
       </c>
       <c r="K75" s="5"/>
       <c r="L75" s="5"/>
-      <c r="M75" s="186"/>
-      <c r="N75" s="171"/>
-      <c r="O75" s="171"/>
-      <c r="P75" s="171"/>
-      <c r="Q75" s="171">
+      <c r="M75" s="164">
+        <v>1.5</v>
+      </c>
+      <c r="N75" s="164">
+        <v>1.5</v>
+      </c>
+      <c r="O75" s="164" t="s">
+        <v>82</v>
+      </c>
+      <c r="P75" s="164">
+        <v>1.0</v>
+      </c>
+      <c r="Q75" s="165">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R75" s="5"/>
       <c r="S75" s="5"/>
@@ -5575,37 +5788,47 @@
     </row>
     <row r="76">
       <c r="A76" s="103"/>
-      <c r="B76" s="187"/>
-      <c r="C76" s="184" t="s">
+      <c r="B76" s="157"/>
+      <c r="C76" s="114" t="s">
         <v>88</v>
       </c>
-      <c r="D76" s="185" t="s">
+      <c r="D76" s="170" t="s">
         <v>52</v>
       </c>
-      <c r="E76" s="182" t="s">
+      <c r="E76" s="52" t="s">
         <v>61</v>
       </c>
-      <c r="F76" s="183">
+      <c r="F76" s="115">
         <v>3.5</v>
       </c>
       <c r="G76" s="103"/>
-      <c r="H76" s="179">
-        <v>0.0</v>
+      <c r="H76" s="46">
+        <f>Q76</f>
+        <v>1.3</v>
       </c>
       <c r="I76" s="103"/>
-      <c r="J76" s="135" t="s">
-        <v>67</v>
+      <c r="J76" s="163" t="s">
+        <v>57</v>
       </c>
       <c r="K76" s="5"/>
       <c r="L76" s="5"/>
-      <c r="M76" s="186"/>
-      <c r="N76" s="171"/>
-      <c r="O76" s="171"/>
-      <c r="P76" s="171"/>
-      <c r="Q76" s="170">
-        <v>0.0</v>
-      </c>
-      <c r="R76" s="135" t="s">
+      <c r="M76" s="164">
+        <v>0.3</v>
+      </c>
+      <c r="N76" s="164">
+        <v>1.0</v>
+      </c>
+      <c r="O76" s="164" t="s">
+        <v>82</v>
+      </c>
+      <c r="P76" s="164" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q76" s="171">
+        <f t="shared" si="15"/>
+        <v>1.3</v>
+      </c>
+      <c r="R76" s="81" t="s">
         <v>112</v>
       </c>
       <c r="S76" s="5"/>
@@ -5624,38 +5847,46 @@
       <c r="AF76" s="5"/>
     </row>
     <row r="77">
-      <c r="A77" s="172"/>
-      <c r="B77" s="162"/>
-      <c r="C77" s="184" t="s">
+      <c r="A77" s="103"/>
+      <c r="B77" s="157"/>
+      <c r="C77" s="114" t="s">
         <v>115</v>
       </c>
       <c r="D77" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="E77" s="182" t="s">
+      <c r="E77" s="52" t="s">
         <v>116</v>
       </c>
-      <c r="F77" s="183">
+      <c r="F77" s="115">
         <v>2.0</v>
       </c>
-      <c r="G77" s="172"/>
+      <c r="G77" s="103"/>
       <c r="H77" s="45">
         <f>SUM(M77:P77)</f>
-        <v>0</v>
-      </c>
-      <c r="I77" s="172"/>
-      <c r="J77" s="135" t="s">
-        <v>67</v>
+        <v>1.2</v>
+      </c>
+      <c r="I77" s="103"/>
+      <c r="J77" s="163" t="s">
+        <v>81</v>
       </c>
       <c r="K77" s="5"/>
       <c r="L77" s="5"/>
-      <c r="M77" s="170"/>
-      <c r="N77" s="174"/>
-      <c r="O77" s="174"/>
-      <c r="P77" s="174"/>
-      <c r="Q77" s="171">
-        <f>SUM(M77:P77)</f>
-        <v>0</v>
+      <c r="M77" s="164">
+        <v>0.4</v>
+      </c>
+      <c r="N77" s="164">
+        <v>0.4</v>
+      </c>
+      <c r="O77" s="164">
+        <v>0.4</v>
+      </c>
+      <c r="P77" s="164" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q77" s="165">
+        <f t="shared" si="15"/>
+        <v>1.2</v>
       </c>
       <c r="R77" s="5"/>
       <c r="S77" s="5"/>
@@ -5674,13 +5905,13 @@
       <c r="AF77" s="5"/>
     </row>
     <row r="78">
-      <c r="A78" s="172"/>
-      <c r="B78" s="163" t="s">
+      <c r="A78" s="103"/>
+      <c r="B78" s="158" t="s">
         <v>71</v>
       </c>
       <c r="C78" s="69"/>
-      <c r="D78" s="164"/>
-      <c r="E78" s="165"/>
+      <c r="D78" s="70"/>
+      <c r="E78" s="104"/>
       <c r="F78" s="69"/>
       <c r="G78" s="105">
         <f>SUM(F79:F81)</f>
@@ -5689,16 +5920,16 @@
       <c r="H78" s="69"/>
       <c r="I78" s="106">
         <f>SUM(H79:H81)</f>
-        <v>0</v>
+        <v>3.1</v>
       </c>
       <c r="J78" s="5"/>
       <c r="K78" s="5"/>
       <c r="L78" s="5"/>
-      <c r="M78" s="165"/>
+      <c r="M78" s="104"/>
       <c r="N78" s="69"/>
-      <c r="O78" s="165"/>
+      <c r="O78" s="104"/>
       <c r="P78" s="69"/>
-      <c r="Q78" s="164"/>
+      <c r="Q78" s="70"/>
       <c r="R78" s="5"/>
       <c r="S78" s="5"/>
       <c r="T78" s="5"/>
@@ -5716,38 +5947,46 @@
       <c r="AF78" s="5"/>
     </row>
     <row r="79">
-      <c r="A79" s="167"/>
-      <c r="B79" s="167"/>
-      <c r="C79" s="188" t="s">
+      <c r="A79" s="160"/>
+      <c r="B79" s="160"/>
+      <c r="C79" s="172" t="s">
         <v>106</v>
       </c>
-      <c r="D79" s="189" t="s">
+      <c r="D79" s="173" t="s">
         <v>107</v>
       </c>
-      <c r="E79" s="190" t="s">
+      <c r="E79" s="174" t="s">
         <v>117</v>
       </c>
-      <c r="F79" s="191">
+      <c r="F79" s="175">
         <v>2.0</v>
       </c>
-      <c r="G79" s="167"/>
+      <c r="G79" s="160"/>
       <c r="H79" s="45">
-        <f t="shared" ref="H79:H82" si="16">SUM(M79:P79)</f>
-        <v>0</v>
-      </c>
-      <c r="I79" s="167"/>
-      <c r="J79" s="135" t="s">
+        <f t="shared" ref="H79:H81" si="16">SUM(M79:P79)</f>
+        <v>1</v>
+      </c>
+      <c r="I79" s="160"/>
+      <c r="J79" s="81" t="s">
         <v>67</v>
       </c>
       <c r="K79" s="5"/>
       <c r="L79" s="5"/>
-      <c r="M79" s="170"/>
-      <c r="N79" s="174"/>
-      <c r="O79" s="174"/>
-      <c r="P79" s="174"/>
-      <c r="Q79" s="171">
-        <f t="shared" ref="Q79:Q82" si="17">SUM(M79:P79)</f>
-        <v>0</v>
+      <c r="M79" s="164">
+        <v>0.5</v>
+      </c>
+      <c r="N79" s="164">
+        <v>0.5</v>
+      </c>
+      <c r="O79" s="164" t="s">
+        <v>82</v>
+      </c>
+      <c r="P79" s="164" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q79" s="165">
+        <f t="shared" ref="Q79:Q96" si="17">SUM(M79:P79)</f>
+        <v>1</v>
       </c>
       <c r="R79" s="5"/>
       <c r="S79" s="5"/>
@@ -5766,38 +6005,46 @@
       <c r="AF79" s="5"/>
     </row>
     <row r="80">
-      <c r="A80" s="192"/>
-      <c r="B80" s="192"/>
-      <c r="C80" s="181" t="s">
+      <c r="A80" s="176"/>
+      <c r="B80" s="176"/>
+      <c r="C80" s="50" t="s">
         <v>96</v>
       </c>
       <c r="D80" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="E80" s="193" t="s">
+      <c r="E80" s="177" t="s">
         <v>118</v>
       </c>
-      <c r="F80" s="183">
+      <c r="F80" s="115">
         <v>2.0</v>
       </c>
-      <c r="G80" s="192"/>
+      <c r="G80" s="176"/>
       <c r="H80" s="45">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="I80" s="192"/>
-      <c r="J80" s="135" t="s">
-        <v>67</v>
+        <v>0.4</v>
+      </c>
+      <c r="I80" s="176"/>
+      <c r="J80" s="163" t="s">
+        <v>57</v>
       </c>
       <c r="K80" s="5"/>
       <c r="L80" s="5"/>
-      <c r="M80" s="170"/>
-      <c r="N80" s="174"/>
-      <c r="O80" s="174"/>
-      <c r="P80" s="174"/>
-      <c r="Q80" s="171">
+      <c r="M80" s="164">
+        <v>0.2</v>
+      </c>
+      <c r="N80" s="164">
+        <v>0.2</v>
+      </c>
+      <c r="O80" s="164" t="s">
+        <v>82</v>
+      </c>
+      <c r="P80" s="164" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q80" s="165">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="R80" s="5"/>
       <c r="S80" s="5"/>
@@ -5816,38 +6063,46 @@
       <c r="AF80" s="5"/>
     </row>
     <row r="81">
-      <c r="A81" s="172"/>
-      <c r="B81" s="172"/>
-      <c r="C81" s="184" t="s">
+      <c r="A81" s="103"/>
+      <c r="B81" s="103"/>
+      <c r="C81" s="114" t="s">
         <v>119</v>
       </c>
       <c r="D81" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="E81" s="193" t="s">
+      <c r="E81" s="177" t="s">
         <v>120</v>
       </c>
-      <c r="F81" s="183">
+      <c r="F81" s="115">
         <v>2.0</v>
       </c>
-      <c r="G81" s="172"/>
+      <c r="G81" s="103"/>
       <c r="H81" s="45">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="I81" s="172"/>
-      <c r="J81" s="135" t="s">
-        <v>67</v>
+        <v>1.7</v>
+      </c>
+      <c r="I81" s="103"/>
+      <c r="J81" s="163" t="s">
+        <v>57</v>
       </c>
       <c r="K81" s="5"/>
       <c r="L81" s="5"/>
-      <c r="M81" s="170"/>
-      <c r="N81" s="174"/>
-      <c r="O81" s="174"/>
-      <c r="P81" s="174"/>
-      <c r="Q81" s="171">
+      <c r="M81" s="164">
+        <v>0.5</v>
+      </c>
+      <c r="N81" s="164">
+        <v>0.5</v>
+      </c>
+      <c r="O81" s="164">
+        <v>0.5</v>
+      </c>
+      <c r="P81" s="164">
+        <v>0.2</v>
+      </c>
+      <c r="Q81" s="165">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>1.7</v>
       </c>
       <c r="R81" s="5"/>
       <c r="S81" s="5"/>
@@ -5866,51 +6121,35 @@
       <c r="AF81" s="5"/>
     </row>
     <row r="82">
-      <c r="A82" s="194" t="s">
-        <v>6</v>
-      </c>
-      <c r="B82" s="194"/>
-      <c r="C82" s="195"/>
-      <c r="D82" s="195"/>
-      <c r="E82" s="196"/>
-      <c r="F82" s="197">
-        <f t="shared" ref="F82:G82" si="18">SUM(F5:F81)</f>
-        <v>216.5</v>
-      </c>
-      <c r="G82" s="198">
-        <f t="shared" si="18"/>
-        <v>216.5</v>
-      </c>
-      <c r="H82" s="199">
-        <f t="shared" si="16"/>
-        <v>73.5</v>
-      </c>
-      <c r="I82" s="198">
-        <f>SUM(I5:I81)</f>
-        <v>73.5</v>
-      </c>
-      <c r="J82" s="200"/>
-      <c r="K82" s="200"/>
-      <c r="L82" s="200"/>
-      <c r="M82" s="199">
-        <f t="shared" ref="M82:P82" si="19">SUM(M5:M81)</f>
-        <v>24.7</v>
-      </c>
-      <c r="N82" s="199">
-        <f t="shared" si="19"/>
-        <v>21.45</v>
-      </c>
-      <c r="O82" s="199">
-        <f t="shared" si="19"/>
-        <v>18.65</v>
-      </c>
-      <c r="P82" s="199">
-        <f t="shared" si="19"/>
-        <v>8.7</v>
-      </c>
-      <c r="Q82" s="199">
+      <c r="A82" s="178" t="s">
+        <v>121</v>
+      </c>
+      <c r="B82" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="C82" s="104"/>
+      <c r="D82" s="69"/>
+      <c r="E82" s="70"/>
+      <c r="F82" s="71"/>
+      <c r="G82" s="105">
+        <f>SUM(F83:F86)</f>
+        <v>5.5</v>
+      </c>
+      <c r="H82" s="71"/>
+      <c r="I82" s="106">
+        <f>SUM(H83:H86)</f>
+        <v>1</v>
+      </c>
+      <c r="J82" s="6"/>
+      <c r="K82" s="6"/>
+      <c r="L82" s="6"/>
+      <c r="M82" s="107"/>
+      <c r="N82" s="107"/>
+      <c r="O82" s="107"/>
+      <c r="P82" s="107"/>
+      <c r="Q82" s="107">
         <f t="shared" si="17"/>
-        <v>73.5</v>
+        <v>0</v>
       </c>
       <c r="R82" s="5"/>
       <c r="S82" s="5"/>
@@ -5929,23 +6168,41 @@
       <c r="AF82" s="5"/>
     </row>
     <row r="83">
-      <c r="A83" s="2"/>
-      <c r="B83" s="2"/>
-      <c r="C83" s="3"/>
-      <c r="D83" s="4"/>
-      <c r="E83" s="5"/>
-      <c r="F83" s="5"/>
-      <c r="G83" s="6"/>
-      <c r="H83" s="5"/>
-      <c r="I83" s="5"/>
-      <c r="J83" s="5"/>
-      <c r="K83" s="5"/>
-      <c r="L83" s="5"/>
-      <c r="M83" s="7"/>
-      <c r="N83" s="7"/>
-      <c r="O83" s="7"/>
-      <c r="P83" s="7"/>
-      <c r="Q83" s="5"/>
+      <c r="A83" s="179"/>
+      <c r="B83" s="180"/>
+      <c r="C83" s="181" t="s">
+        <v>80</v>
+      </c>
+      <c r="D83" s="60" t="s">
+        <v>20</v>
+      </c>
+      <c r="E83" s="182" t="s">
+        <v>21</v>
+      </c>
+      <c r="F83" s="183">
+        <v>2.0</v>
+      </c>
+      <c r="G83" s="184"/>
+      <c r="H83" s="64">
+        <f t="shared" ref="H83:H86" si="18">SUM(M83:P83)</f>
+        <v>0.5</v>
+      </c>
+      <c r="I83" s="185"/>
+      <c r="J83" s="163" t="s">
+        <v>54</v>
+      </c>
+      <c r="K83" s="186"/>
+      <c r="L83" s="186"/>
+      <c r="M83" s="187">
+        <v>0.5</v>
+      </c>
+      <c r="N83" s="188"/>
+      <c r="O83" s="188"/>
+      <c r="P83" s="188"/>
+      <c r="Q83" s="130">
+        <f t="shared" si="17"/>
+        <v>0.5</v>
+      </c>
       <c r="R83" s="5"/>
       <c r="S83" s="5"/>
       <c r="T83" s="5"/>
@@ -5963,23 +6220,43 @@
       <c r="AF83" s="5"/>
     </row>
     <row r="84">
-      <c r="A84" s="2"/>
-      <c r="B84" s="2"/>
-      <c r="C84" s="3"/>
-      <c r="D84" s="4"/>
-      <c r="E84" s="5"/>
-      <c r="F84" s="5"/>
-      <c r="G84" s="6"/>
-      <c r="H84" s="5"/>
-      <c r="I84" s="5"/>
-      <c r="J84" s="5"/>
-      <c r="K84" s="5"/>
-      <c r="L84" s="5"/>
-      <c r="M84" s="7"/>
-      <c r="N84" s="7"/>
-      <c r="O84" s="7"/>
-      <c r="P84" s="7"/>
-      <c r="Q84" s="5"/>
+      <c r="A84" s="189"/>
+      <c r="B84" s="190"/>
+      <c r="C84" s="191" t="s">
+        <v>83</v>
+      </c>
+      <c r="D84" s="75" t="s">
+        <v>20</v>
+      </c>
+      <c r="E84" s="132" t="s">
+        <v>122</v>
+      </c>
+      <c r="F84" s="192">
+        <v>1.0</v>
+      </c>
+      <c r="G84" s="193"/>
+      <c r="H84" s="134">
+        <f t="shared" si="18"/>
+        <v>0.5</v>
+      </c>
+      <c r="I84" s="193"/>
+      <c r="J84" s="163" t="s">
+        <v>54</v>
+      </c>
+      <c r="K84" s="186"/>
+      <c r="L84" s="186"/>
+      <c r="M84" s="135">
+        <v>0.25</v>
+      </c>
+      <c r="N84" s="135">
+        <v>0.25</v>
+      </c>
+      <c r="O84" s="135"/>
+      <c r="P84" s="135"/>
+      <c r="Q84" s="101">
+        <f t="shared" si="17"/>
+        <v>0.5</v>
+      </c>
       <c r="R84" s="5"/>
       <c r="S84" s="5"/>
       <c r="T84" s="5"/>
@@ -5997,23 +6274,39 @@
       <c r="AF84" s="5"/>
     </row>
     <row r="85">
-      <c r="A85" s="2"/>
-      <c r="B85" s="2"/>
-      <c r="C85" s="3"/>
-      <c r="D85" s="4"/>
-      <c r="E85" s="5"/>
-      <c r="F85" s="5"/>
-      <c r="G85" s="6"/>
-      <c r="H85" s="5"/>
-      <c r="I85" s="5"/>
-      <c r="J85" s="5"/>
-      <c r="K85" s="5"/>
-      <c r="L85" s="5"/>
-      <c r="M85" s="7"/>
-      <c r="N85" s="7"/>
-      <c r="O85" s="7"/>
-      <c r="P85" s="7"/>
-      <c r="Q85" s="5"/>
+      <c r="A85" s="189"/>
+      <c r="B85" s="190"/>
+      <c r="C85" s="194" t="s">
+        <v>123</v>
+      </c>
+      <c r="D85" s="75" t="s">
+        <v>52</v>
+      </c>
+      <c r="E85" s="195" t="s">
+        <v>61</v>
+      </c>
+      <c r="F85" s="192">
+        <v>1.0</v>
+      </c>
+      <c r="G85" s="193"/>
+      <c r="H85" s="134">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="I85" s="193"/>
+      <c r="J85" s="163" t="s">
+        <v>67</v>
+      </c>
+      <c r="K85" s="186"/>
+      <c r="L85" s="186"/>
+      <c r="M85" s="135"/>
+      <c r="N85" s="135"/>
+      <c r="O85" s="135"/>
+      <c r="P85" s="135"/>
+      <c r="Q85" s="101">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
       <c r="R85" s="5"/>
       <c r="S85" s="5"/>
       <c r="T85" s="5"/>
@@ -6031,23 +6324,39 @@
       <c r="AF85" s="5"/>
     </row>
     <row r="86">
-      <c r="A86" s="2"/>
-      <c r="B86" s="2"/>
-      <c r="C86" s="3"/>
-      <c r="D86" s="4"/>
-      <c r="E86" s="5"/>
-      <c r="F86" s="5"/>
-      <c r="G86" s="6"/>
-      <c r="H86" s="5"/>
-      <c r="I86" s="5"/>
-      <c r="J86" s="5"/>
-      <c r="K86" s="5"/>
-      <c r="L86" s="5"/>
-      <c r="M86" s="7"/>
-      <c r="N86" s="7"/>
-      <c r="O86" s="7"/>
-      <c r="P86" s="7"/>
-      <c r="Q86" s="5"/>
+      <c r="A86" s="189"/>
+      <c r="B86" s="196"/>
+      <c r="C86" s="197" t="s">
+        <v>124</v>
+      </c>
+      <c r="D86" s="89" t="s">
+        <v>52</v>
+      </c>
+      <c r="E86" s="198" t="s">
+        <v>64</v>
+      </c>
+      <c r="F86" s="199">
+        <v>1.5</v>
+      </c>
+      <c r="G86" s="200"/>
+      <c r="H86" s="140">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="I86" s="200"/>
+      <c r="J86" s="163" t="s">
+        <v>67</v>
+      </c>
+      <c r="K86" s="186"/>
+      <c r="L86" s="186"/>
+      <c r="M86" s="201"/>
+      <c r="N86" s="201"/>
+      <c r="O86" s="202"/>
+      <c r="P86" s="202"/>
+      <c r="Q86" s="142">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
       <c r="R86" s="5"/>
       <c r="S86" s="5"/>
       <c r="T86" s="5"/>
@@ -6065,23 +6374,34 @@
       <c r="AF86" s="5"/>
     </row>
     <row r="87">
-      <c r="A87" s="2"/>
-      <c r="B87" s="2"/>
-      <c r="C87" s="3"/>
-      <c r="D87" s="4"/>
-      <c r="E87" s="5"/>
-      <c r="F87" s="5"/>
-      <c r="G87" s="6"/>
-      <c r="H87" s="5"/>
-      <c r="I87" s="5"/>
-      <c r="J87" s="5"/>
-      <c r="K87" s="5"/>
-      <c r="L87" s="5"/>
-      <c r="M87" s="7"/>
-      <c r="N87" s="7"/>
-      <c r="O87" s="7"/>
-      <c r="P87" s="7"/>
-      <c r="Q87" s="5"/>
+      <c r="A87" s="189"/>
+      <c r="B87" s="203" t="s">
+        <v>50</v>
+      </c>
+      <c r="C87" s="204"/>
+      <c r="D87" s="69"/>
+      <c r="E87" s="205"/>
+      <c r="F87" s="98"/>
+      <c r="G87" s="105">
+        <f>SUM(F88:F92)</f>
+        <v>6.5</v>
+      </c>
+      <c r="H87" s="98"/>
+      <c r="I87" s="106">
+        <f>SUM(H88:H92)</f>
+        <v>0</v>
+      </c>
+      <c r="J87" s="163"/>
+      <c r="K87" s="186"/>
+      <c r="L87" s="186"/>
+      <c r="M87" s="206"/>
+      <c r="N87" s="206"/>
+      <c r="O87" s="206"/>
+      <c r="P87" s="206"/>
+      <c r="Q87" s="107">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
       <c r="R87" s="5"/>
       <c r="S87" s="5"/>
       <c r="T87" s="5"/>
@@ -6099,23 +6419,39 @@
       <c r="AF87" s="5"/>
     </row>
     <row r="88">
-      <c r="A88" s="2"/>
-      <c r="B88" s="2"/>
-      <c r="C88" s="3"/>
-      <c r="D88" s="4"/>
-      <c r="E88" s="5"/>
-      <c r="F88" s="5"/>
-      <c r="G88" s="6"/>
-      <c r="H88" s="5"/>
-      <c r="I88" s="5"/>
-      <c r="J88" s="5"/>
-      <c r="K88" s="5"/>
-      <c r="L88" s="5"/>
-      <c r="M88" s="7"/>
-      <c r="N88" s="7"/>
-      <c r="O88" s="7"/>
-      <c r="P88" s="7"/>
-      <c r="Q88" s="5"/>
+      <c r="A88" s="189"/>
+      <c r="B88" s="190"/>
+      <c r="C88" s="191" t="s">
+        <v>89</v>
+      </c>
+      <c r="D88" s="75" t="s">
+        <v>52</v>
+      </c>
+      <c r="E88" s="195" t="s">
+        <v>64</v>
+      </c>
+      <c r="F88" s="192">
+        <v>1.0</v>
+      </c>
+      <c r="G88" s="193"/>
+      <c r="H88" s="134">
+        <f t="shared" ref="H88:H92" si="19">SUM(M88:P88)</f>
+        <v>0</v>
+      </c>
+      <c r="I88" s="193"/>
+      <c r="J88" s="163" t="s">
+        <v>67</v>
+      </c>
+      <c r="K88" s="186"/>
+      <c r="L88" s="186"/>
+      <c r="M88" s="207"/>
+      <c r="N88" s="135"/>
+      <c r="O88" s="207"/>
+      <c r="P88" s="207"/>
+      <c r="Q88" s="101">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
       <c r="R88" s="5"/>
       <c r="S88" s="5"/>
       <c r="T88" s="5"/>
@@ -6133,23 +6469,39 @@
       <c r="AF88" s="5"/>
     </row>
     <row r="89">
-      <c r="A89" s="2"/>
-      <c r="B89" s="2"/>
-      <c r="C89" s="3"/>
-      <c r="D89" s="4"/>
-      <c r="E89" s="5"/>
-      <c r="F89" s="5"/>
-      <c r="G89" s="6"/>
-      <c r="H89" s="5"/>
-      <c r="I89" s="5"/>
-      <c r="J89" s="5"/>
-      <c r="K89" s="5"/>
-      <c r="L89" s="5"/>
-      <c r="M89" s="7"/>
-      <c r="N89" s="7"/>
-      <c r="O89" s="7"/>
-      <c r="P89" s="7"/>
-      <c r="Q89" s="5"/>
+      <c r="A89" s="189"/>
+      <c r="B89" s="190"/>
+      <c r="C89" s="194" t="s">
+        <v>125</v>
+      </c>
+      <c r="D89" s="75" t="s">
+        <v>52</v>
+      </c>
+      <c r="E89" s="132" t="s">
+        <v>126</v>
+      </c>
+      <c r="F89" s="192">
+        <v>2.0</v>
+      </c>
+      <c r="G89" s="193"/>
+      <c r="H89" s="134">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="I89" s="193"/>
+      <c r="J89" s="163" t="s">
+        <v>67</v>
+      </c>
+      <c r="K89" s="186"/>
+      <c r="L89" s="186"/>
+      <c r="M89" s="135"/>
+      <c r="N89" s="207"/>
+      <c r="O89" s="207"/>
+      <c r="P89" s="135"/>
+      <c r="Q89" s="101">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
       <c r="R89" s="5"/>
       <c r="S89" s="5"/>
       <c r="T89" s="5"/>
@@ -6167,23 +6519,39 @@
       <c r="AF89" s="5"/>
     </row>
     <row r="90">
-      <c r="A90" s="2"/>
-      <c r="B90" s="2"/>
-      <c r="C90" s="3"/>
-      <c r="D90" s="4"/>
-      <c r="E90" s="5"/>
-      <c r="F90" s="5"/>
-      <c r="G90" s="6"/>
-      <c r="H90" s="5"/>
-      <c r="I90" s="5"/>
-      <c r="J90" s="5"/>
-      <c r="K90" s="5"/>
-      <c r="L90" s="5"/>
-      <c r="M90" s="7"/>
-      <c r="N90" s="7"/>
-      <c r="O90" s="7"/>
-      <c r="P90" s="7"/>
-      <c r="Q90" s="5"/>
+      <c r="A90" s="189"/>
+      <c r="B90" s="190"/>
+      <c r="C90" s="194" t="s">
+        <v>127</v>
+      </c>
+      <c r="D90" s="75" t="s">
+        <v>52</v>
+      </c>
+      <c r="E90" s="195" t="s">
+        <v>66</v>
+      </c>
+      <c r="F90" s="192">
+        <v>1.0</v>
+      </c>
+      <c r="G90" s="193"/>
+      <c r="H90" s="134">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="I90" s="193"/>
+      <c r="J90" s="163" t="s">
+        <v>67</v>
+      </c>
+      <c r="K90" s="186"/>
+      <c r="L90" s="186"/>
+      <c r="M90" s="207"/>
+      <c r="N90" s="207"/>
+      <c r="O90" s="207"/>
+      <c r="P90" s="135"/>
+      <c r="Q90" s="101">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
       <c r="R90" s="5"/>
       <c r="S90" s="5"/>
       <c r="T90" s="5"/>
@@ -6201,23 +6569,39 @@
       <c r="AF90" s="5"/>
     </row>
     <row r="91">
-      <c r="A91" s="2"/>
-      <c r="B91" s="2"/>
-      <c r="C91" s="3"/>
-      <c r="D91" s="4"/>
-      <c r="E91" s="5"/>
-      <c r="F91" s="5"/>
-      <c r="G91" s="6"/>
-      <c r="H91" s="5"/>
-      <c r="I91" s="5"/>
-      <c r="J91" s="5"/>
-      <c r="K91" s="5"/>
-      <c r="L91" s="5"/>
-      <c r="M91" s="7"/>
-      <c r="N91" s="7"/>
-      <c r="O91" s="7"/>
-      <c r="P91" s="7"/>
-      <c r="Q91" s="5"/>
+      <c r="A91" s="189"/>
+      <c r="B91" s="190"/>
+      <c r="C91" s="194" t="s">
+        <v>128</v>
+      </c>
+      <c r="D91" s="75" t="s">
+        <v>52</v>
+      </c>
+      <c r="E91" s="195" t="s">
+        <v>61</v>
+      </c>
+      <c r="F91" s="192">
+        <v>1.5</v>
+      </c>
+      <c r="G91" s="193"/>
+      <c r="H91" s="134">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="I91" s="193"/>
+      <c r="J91" s="163" t="s">
+        <v>67</v>
+      </c>
+      <c r="K91" s="186"/>
+      <c r="L91" s="186"/>
+      <c r="M91" s="207"/>
+      <c r="N91" s="207"/>
+      <c r="O91" s="207"/>
+      <c r="P91" s="135"/>
+      <c r="Q91" s="101">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
       <c r="R91" s="5"/>
       <c r="S91" s="5"/>
       <c r="T91" s="5"/>
@@ -6235,23 +6619,39 @@
       <c r="AF91" s="5"/>
     </row>
     <row r="92">
-      <c r="A92" s="2"/>
-      <c r="B92" s="2"/>
-      <c r="C92" s="3"/>
-      <c r="D92" s="4"/>
-      <c r="E92" s="5"/>
-      <c r="F92" s="5"/>
-      <c r="G92" s="6"/>
-      <c r="H92" s="5"/>
-      <c r="I92" s="5"/>
-      <c r="J92" s="5"/>
-      <c r="K92" s="5"/>
-      <c r="L92" s="5"/>
-      <c r="M92" s="7"/>
-      <c r="N92" s="7"/>
-      <c r="O92" s="7"/>
-      <c r="P92" s="7"/>
-      <c r="Q92" s="5"/>
+      <c r="A92" s="189"/>
+      <c r="B92" s="196"/>
+      <c r="C92" s="208" t="s">
+        <v>69</v>
+      </c>
+      <c r="D92" s="89" t="s">
+        <v>52</v>
+      </c>
+      <c r="E92" s="138" t="s">
+        <v>129</v>
+      </c>
+      <c r="F92" s="199">
+        <v>1.0</v>
+      </c>
+      <c r="G92" s="200"/>
+      <c r="H92" s="140">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="I92" s="200"/>
+      <c r="J92" s="163" t="s">
+        <v>67</v>
+      </c>
+      <c r="K92" s="186"/>
+      <c r="L92" s="186"/>
+      <c r="M92" s="202"/>
+      <c r="N92" s="202"/>
+      <c r="O92" s="202"/>
+      <c r="P92" s="202"/>
+      <c r="Q92" s="142">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
       <c r="R92" s="5"/>
       <c r="S92" s="5"/>
       <c r="T92" s="5"/>
@@ -6269,23 +6669,34 @@
       <c r="AF92" s="5"/>
     </row>
     <row r="93">
-      <c r="A93" s="2"/>
-      <c r="B93" s="2"/>
-      <c r="C93" s="3"/>
-      <c r="D93" s="4"/>
-      <c r="E93" s="5"/>
-      <c r="F93" s="5"/>
-      <c r="G93" s="6"/>
-      <c r="H93" s="5"/>
-      <c r="I93" s="5"/>
-      <c r="J93" s="5"/>
-      <c r="K93" s="5"/>
-      <c r="L93" s="5"/>
-      <c r="M93" s="7"/>
-      <c r="N93" s="7"/>
-      <c r="O93" s="7"/>
-      <c r="P93" s="7"/>
-      <c r="Q93" s="5"/>
+      <c r="A93" s="189"/>
+      <c r="B93" s="209" t="s">
+        <v>71</v>
+      </c>
+      <c r="C93" s="210"/>
+      <c r="D93" s="146"/>
+      <c r="E93" s="211"/>
+      <c r="F93" s="148"/>
+      <c r="G93" s="149">
+        <f>SUM(F94:F95)</f>
+        <v>7</v>
+      </c>
+      <c r="H93" s="148"/>
+      <c r="I93" s="150">
+        <f>SUM(H94:H95)</f>
+        <v>0</v>
+      </c>
+      <c r="J93" s="163"/>
+      <c r="K93" s="186"/>
+      <c r="L93" s="186"/>
+      <c r="M93" s="212"/>
+      <c r="N93" s="212"/>
+      <c r="O93" s="212"/>
+      <c r="P93" s="212"/>
+      <c r="Q93" s="151">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
       <c r="R93" s="5"/>
       <c r="S93" s="5"/>
       <c r="T93" s="5"/>
@@ -6303,23 +6714,39 @@
       <c r="AF93" s="5"/>
     </row>
     <row r="94">
-      <c r="A94" s="2"/>
-      <c r="B94" s="2"/>
-      <c r="C94" s="3"/>
-      <c r="D94" s="4"/>
-      <c r="E94" s="5"/>
-      <c r="F94" s="5"/>
-      <c r="G94" s="6"/>
-      <c r="H94" s="5"/>
-      <c r="I94" s="5"/>
-      <c r="J94" s="5"/>
-      <c r="K94" s="5"/>
-      <c r="L94" s="5"/>
-      <c r="M94" s="7"/>
-      <c r="N94" s="7"/>
-      <c r="O94" s="7"/>
-      <c r="P94" s="7"/>
-      <c r="Q94" s="5"/>
+      <c r="A94" s="179"/>
+      <c r="B94" s="180"/>
+      <c r="C94" s="213" t="s">
+        <v>130</v>
+      </c>
+      <c r="D94" s="60" t="s">
+        <v>107</v>
+      </c>
+      <c r="E94" s="152" t="s">
+        <v>131</v>
+      </c>
+      <c r="F94" s="153">
+        <v>6.0</v>
+      </c>
+      <c r="G94" s="184"/>
+      <c r="H94" s="154">
+        <f t="shared" ref="H94:H96" si="20">SUM(M94:P94)</f>
+        <v>0</v>
+      </c>
+      <c r="I94" s="185"/>
+      <c r="J94" s="163" t="s">
+        <v>67</v>
+      </c>
+      <c r="K94" s="186"/>
+      <c r="L94" s="186"/>
+      <c r="M94" s="187"/>
+      <c r="N94" s="187"/>
+      <c r="O94" s="188"/>
+      <c r="P94" s="188"/>
+      <c r="Q94" s="130">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
       <c r="R94" s="5"/>
       <c r="S94" s="5"/>
       <c r="T94" s="5"/>
@@ -6337,23 +6764,39 @@
       <c r="AF94" s="5"/>
     </row>
     <row r="95">
-      <c r="A95" s="2"/>
-      <c r="B95" s="2"/>
-      <c r="C95" s="3"/>
-      <c r="D95" s="4"/>
-      <c r="E95" s="5"/>
-      <c r="F95" s="5"/>
-      <c r="G95" s="6"/>
-      <c r="H95" s="5"/>
-      <c r="I95" s="5"/>
-      <c r="J95" s="5"/>
-      <c r="K95" s="5"/>
-      <c r="L95" s="5"/>
-      <c r="M95" s="7"/>
-      <c r="N95" s="7"/>
-      <c r="O95" s="7"/>
-      <c r="P95" s="7"/>
-      <c r="Q95" s="5"/>
+      <c r="A95" s="214"/>
+      <c r="B95" s="196"/>
+      <c r="C95" s="208" t="s">
+        <v>96</v>
+      </c>
+      <c r="D95" s="89" t="s">
+        <v>74</v>
+      </c>
+      <c r="E95" s="156" t="s">
+        <v>132</v>
+      </c>
+      <c r="F95" s="199">
+        <v>1.0</v>
+      </c>
+      <c r="G95" s="200"/>
+      <c r="H95" s="140">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I95" s="200"/>
+      <c r="J95" s="163" t="s">
+        <v>67</v>
+      </c>
+      <c r="K95" s="186"/>
+      <c r="L95" s="186"/>
+      <c r="M95" s="201"/>
+      <c r="N95" s="202"/>
+      <c r="O95" s="202"/>
+      <c r="P95" s="201"/>
+      <c r="Q95" s="142">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
       <c r="R95" s="5"/>
       <c r="S95" s="5"/>
       <c r="T95" s="5"/>
@@ -6371,23 +6814,52 @@
       <c r="AF95" s="5"/>
     </row>
     <row r="96">
-      <c r="A96" s="2"/>
-      <c r="B96" s="2"/>
-      <c r="C96" s="3"/>
-      <c r="D96" s="4"/>
-      <c r="E96" s="5"/>
-      <c r="F96" s="5"/>
-      <c r="G96" s="6"/>
-      <c r="H96" s="5"/>
-      <c r="I96" s="5"/>
-      <c r="J96" s="5"/>
-      <c r="K96" s="5"/>
-      <c r="L96" s="5"/>
-      <c r="M96" s="7"/>
-      <c r="N96" s="7"/>
-      <c r="O96" s="7"/>
-      <c r="P96" s="7"/>
-      <c r="Q96" s="5"/>
+      <c r="A96" s="215" t="s">
+        <v>6</v>
+      </c>
+      <c r="B96" s="215"/>
+      <c r="C96" s="216"/>
+      <c r="D96" s="216"/>
+      <c r="E96" s="217"/>
+      <c r="F96" s="218">
+        <f t="shared" ref="F96:G96" si="21">SUM(F5:F95)</f>
+        <v>235.5</v>
+      </c>
+      <c r="G96" s="219">
+        <f t="shared" si="21"/>
+        <v>235.5</v>
+      </c>
+      <c r="H96" s="220">
+        <f t="shared" si="20"/>
+        <v>100.9</v>
+      </c>
+      <c r="I96" s="219">
+        <f>SUM(I5:I95)</f>
+        <v>100.9</v>
+      </c>
+      <c r="J96" s="221"/>
+      <c r="K96" s="221"/>
+      <c r="L96" s="221"/>
+      <c r="M96" s="220">
+        <f t="shared" ref="M96:P96" si="22">SUM(M5:M95)</f>
+        <v>37.15</v>
+      </c>
+      <c r="N96" s="220">
+        <f t="shared" si="22"/>
+        <v>31.8</v>
+      </c>
+      <c r="O96" s="220">
+        <f t="shared" si="22"/>
+        <v>21.55</v>
+      </c>
+      <c r="P96" s="220">
+        <f t="shared" si="22"/>
+        <v>10.4</v>
+      </c>
+      <c r="Q96" s="220">
+        <f t="shared" si="17"/>
+        <v>100.9</v>
+      </c>
       <c r="R96" s="5"/>
       <c r="S96" s="5"/>
       <c r="T96" s="5"/>
@@ -6439,23 +6911,6 @@
       <c r="AF97" s="5"/>
     </row>
     <row r="98">
-      <c r="A98" s="2"/>
-      <c r="B98" s="2"/>
-      <c r="C98" s="3"/>
-      <c r="D98" s="4"/>
-      <c r="E98" s="5"/>
-      <c r="F98" s="5"/>
-      <c r="G98" s="6"/>
-      <c r="H98" s="5"/>
-      <c r="I98" s="5"/>
-      <c r="J98" s="5"/>
-      <c r="K98" s="5"/>
-      <c r="L98" s="5"/>
-      <c r="M98" s="7"/>
-      <c r="N98" s="7"/>
-      <c r="O98" s="7"/>
-      <c r="P98" s="7"/>
-      <c r="Q98" s="5"/>
       <c r="R98" s="5"/>
       <c r="S98" s="5"/>
       <c r="T98" s="5"/>
@@ -37184,7 +37639,7 @@
       <c r="G1002" s="6"/>
       <c r="H1002" s="5"/>
       <c r="I1002" s="5"/>
-      <c r="J1002" s="201"/>
+      <c r="J1002" s="5"/>
       <c r="K1002" s="5"/>
       <c r="L1002" s="5"/>
       <c r="M1002" s="7"/>
@@ -37209,7 +37664,7 @@
       <c r="AF1002" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I5:I64 M5:Q64 M66:Q68 M70:Q77 M79:Q82 I82">
+  <conditionalFormatting sqref="I5:I64 M5:Q64 M66:Q68 M70:Q77 M79:Q96 I82:I96">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Update Iteration 5 documents
</commit_message>
<xml_diff>
--- a/documentation/CS451R.Group14.EffortEstimate.xlsx
+++ b/documentation/CS451R.Group14.EffortEstimate.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="133">
   <si>
     <t>Note: Beyond Iteration 2, nothing is changed.</t>
   </si>
@@ -688,7 +688,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="11">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -734,20 +734,10 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="10.0"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <sz val="12.0"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
-      <sz val="12.0"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10.0"/>
       <name val="Arial"/>
     </font>
@@ -936,7 +926,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="222">
+  <cellXfs count="186">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1342,9 +1332,6 @@
     <xf borderId="10" fillId="5" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="5" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
     <xf borderId="11" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
@@ -1426,10 +1413,7 @@
     <xf borderId="13" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="3" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -1444,14 +1428,8 @@
     <xf borderId="13" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="13" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
     <xf borderId="5" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="2" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -1471,137 +1449,41 @@
     <xf borderId="5" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="13" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="13" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="13" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="1" fillId="5" fontId="9" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="3" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="5" fontId="9" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="5" fontId="9" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="9" fillId="6" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="7" fillId="6" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="6" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="6" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="3" fillId="5" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="6" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="9" fillId="6" fontId="10" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="13" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="10" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="11" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="10" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="12" fillId="5" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="11" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="11" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="5" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="5" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="5" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="9" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="4" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="10" fillId="5" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="2" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="14" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="6" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="7" fillId="6" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="6" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="9" fillId="6" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="6" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="9" fillId="6" fontId="12" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4592,7 +4474,7 @@
       <c r="O53" s="100">
         <v>0.3</v>
       </c>
-      <c r="P53" s="135">
+      <c r="P53" s="100">
         <v>0.0</v>
       </c>
       <c r="Q53" s="101">
@@ -4618,7 +4500,7 @@
     <row r="54" ht="15.0" customHeight="1">
       <c r="A54" s="67"/>
       <c r="B54" s="86"/>
-      <c r="C54" s="136" t="s">
+      <c r="C54" s="135" t="s">
         <v>88</v>
       </c>
       <c r="D54" s="75" t="s">
@@ -4641,16 +4523,16 @@
       </c>
       <c r="K54" s="5"/>
       <c r="L54" s="5"/>
-      <c r="M54" s="135">
+      <c r="M54" s="100">
         <v>0.0</v>
       </c>
-      <c r="N54" s="135">
+      <c r="N54" s="100">
         <v>0.0</v>
       </c>
-      <c r="O54" s="135">
+      <c r="O54" s="100">
         <v>0.0</v>
       </c>
-      <c r="P54" s="135">
+      <c r="P54" s="100">
         <v>0.0</v>
       </c>
       <c r="Q54" s="101">
@@ -4678,20 +4560,20 @@
     <row r="55" ht="35.25" customHeight="1">
       <c r="A55" s="67"/>
       <c r="B55" s="87"/>
-      <c r="C55" s="137" t="s">
+      <c r="C55" s="136" t="s">
         <v>101</v>
       </c>
       <c r="D55" s="89" t="s">
         <v>52</v>
       </c>
-      <c r="E55" s="138" t="s">
+      <c r="E55" s="137" t="s">
         <v>64</v>
       </c>
-      <c r="F55" s="139">
+      <c r="F55" s="138">
         <v>3.0</v>
       </c>
       <c r="G55" s="92"/>
-      <c r="H55" s="140">
+      <c r="H55" s="139">
         <f t="shared" si="9"/>
         <v>1.5</v>
       </c>
@@ -4701,15 +4583,15 @@
       </c>
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
-      <c r="M55" s="141">
+      <c r="M55" s="140">
         <v>0.5</v>
       </c>
-      <c r="N55" s="141">
+      <c r="N55" s="140">
         <v>1.0</v>
       </c>
-      <c r="O55" s="142"/>
-      <c r="P55" s="142"/>
-      <c r="Q55" s="142">
+      <c r="O55" s="141"/>
+      <c r="P55" s="141"/>
+      <c r="Q55" s="141">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
@@ -4854,7 +4736,7 @@
       </c>
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
-      <c r="M58" s="135"/>
+      <c r="M58" s="100"/>
       <c r="N58" s="101"/>
       <c r="O58" s="101"/>
       <c r="P58" s="100"/>
@@ -4981,20 +4863,20 @@
     <row r="61" ht="15.0" customHeight="1">
       <c r="A61" s="67"/>
       <c r="B61" s="87"/>
-      <c r="C61" s="143" t="s">
+      <c r="C61" s="142" t="s">
         <v>69</v>
       </c>
       <c r="D61" s="89" t="s">
         <v>52</v>
       </c>
-      <c r="E61" s="138" t="s">
+      <c r="E61" s="137" t="s">
         <v>61</v>
       </c>
-      <c r="F61" s="139">
+      <c r="F61" s="138">
         <v>1.5</v>
       </c>
       <c r="G61" s="92"/>
-      <c r="H61" s="140">
+      <c r="H61" s="139">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -5004,11 +4886,11 @@
       </c>
       <c r="K61" s="5"/>
       <c r="L61" s="5"/>
-      <c r="M61" s="142"/>
-      <c r="N61" s="142"/>
-      <c r="O61" s="142"/>
-      <c r="P61" s="142"/>
-      <c r="Q61" s="142">
+      <c r="M61" s="141"/>
+      <c r="N61" s="141"/>
+      <c r="O61" s="141"/>
+      <c r="P61" s="141"/>
+      <c r="Q61" s="141">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5030,30 +4912,30 @@
     </row>
     <row r="62" ht="15.0" customHeight="1">
       <c r="A62" s="67"/>
-      <c r="B62" s="144" t="s">
+      <c r="B62" s="143" t="s">
         <v>71</v>
       </c>
-      <c r="C62" s="145"/>
-      <c r="D62" s="146"/>
-      <c r="E62" s="147"/>
-      <c r="F62" s="148"/>
-      <c r="G62" s="149">
+      <c r="C62" s="144"/>
+      <c r="D62" s="145"/>
+      <c r="E62" s="146"/>
+      <c r="F62" s="147"/>
+      <c r="G62" s="148">
         <f>SUM(F63:F64)</f>
         <v>4</v>
       </c>
-      <c r="H62" s="148"/>
-      <c r="I62" s="150">
+      <c r="H62" s="147"/>
+      <c r="I62" s="149">
         <f>SUM(H63:H64)</f>
         <v>0</v>
       </c>
       <c r="J62" s="5"/>
       <c r="K62" s="5"/>
       <c r="L62" s="5"/>
-      <c r="M62" s="151"/>
-      <c r="N62" s="151"/>
-      <c r="O62" s="151"/>
-      <c r="P62" s="151"/>
-      <c r="Q62" s="151">
+      <c r="M62" s="150"/>
+      <c r="N62" s="150"/>
+      <c r="O62" s="150"/>
+      <c r="P62" s="150"/>
+      <c r="Q62" s="150">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5082,14 +4964,14 @@
       <c r="D63" s="60" t="s">
         <v>107</v>
       </c>
-      <c r="E63" s="152" t="s">
+      <c r="E63" s="151" t="s">
         <v>108</v>
       </c>
-      <c r="F63" s="153">
+      <c r="F63" s="152">
         <v>2.0</v>
       </c>
       <c r="G63" s="127"/>
-      <c r="H63" s="154">
+      <c r="H63" s="153">
         <f t="shared" ref="H63:H64" si="11">SUM(M63:P63)</f>
         <v>0</v>
       </c>
@@ -5124,22 +5006,22 @@
       <c r="AF63" s="5"/>
     </row>
     <row r="64" ht="15.0" customHeight="1">
-      <c r="A64" s="155"/>
+      <c r="A64" s="154"/>
       <c r="B64" s="87"/>
-      <c r="C64" s="143" t="s">
+      <c r="C64" s="142" t="s">
         <v>96</v>
       </c>
       <c r="D64" s="89" t="s">
         <v>74</v>
       </c>
-      <c r="E64" s="156" t="s">
+      <c r="E64" s="155" t="s">
         <v>109</v>
       </c>
-      <c r="F64" s="139">
+      <c r="F64" s="138">
         <v>2.0</v>
       </c>
       <c r="G64" s="92"/>
-      <c r="H64" s="140">
+      <c r="H64" s="139">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -5149,11 +5031,11 @@
       </c>
       <c r="K64" s="5"/>
       <c r="L64" s="5"/>
-      <c r="M64" s="141"/>
-      <c r="N64" s="142"/>
-      <c r="O64" s="142"/>
-      <c r="P64" s="141"/>
-      <c r="Q64" s="142">
+      <c r="M64" s="140"/>
+      <c r="N64" s="141"/>
+      <c r="O64" s="141"/>
+      <c r="P64" s="140"/>
+      <c r="Q64" s="141">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5174,10 +5056,10 @@
       <c r="AF64" s="5"/>
     </row>
     <row r="65" ht="18.75" customHeight="1">
-      <c r="A65" s="157" t="s">
+      <c r="A65" s="156" t="s">
         <v>110</v>
       </c>
-      <c r="B65" s="158" t="s">
+      <c r="B65" s="157" t="s">
         <v>79</v>
       </c>
       <c r="C65" s="69"/>
@@ -5198,61 +5080,61 @@
       <c r="O65" s="104"/>
       <c r="P65" s="69"/>
       <c r="Q65" s="70"/>
-      <c r="R65" s="159"/>
-      <c r="S65" s="159"/>
-      <c r="T65" s="159"/>
-      <c r="U65" s="159"/>
-      <c r="V65" s="159"/>
-      <c r="W65" s="159"/>
-      <c r="X65" s="159"/>
-      <c r="Y65" s="159"/>
-      <c r="Z65" s="159"/>
-      <c r="AA65" s="159"/>
-      <c r="AB65" s="159"/>
-      <c r="AC65" s="159"/>
-      <c r="AD65" s="159"/>
-      <c r="AE65" s="159"/>
-      <c r="AF65" s="159"/>
+      <c r="R65" s="158"/>
+      <c r="S65" s="158"/>
+      <c r="T65" s="158"/>
+      <c r="U65" s="158"/>
+      <c r="V65" s="158"/>
+      <c r="W65" s="158"/>
+      <c r="X65" s="158"/>
+      <c r="Y65" s="158"/>
+      <c r="Z65" s="158"/>
+      <c r="AA65" s="158"/>
+      <c r="AB65" s="158"/>
+      <c r="AC65" s="158"/>
+      <c r="AD65" s="158"/>
+      <c r="AE65" s="158"/>
+      <c r="AF65" s="158"/>
     </row>
     <row r="66" ht="16.5" customHeight="1">
-      <c r="A66" s="160"/>
-      <c r="B66" s="160"/>
-      <c r="C66" s="160" t="s">
+      <c r="A66" s="159"/>
+      <c r="B66" s="159"/>
+      <c r="C66" s="159" t="s">
         <v>80</v>
       </c>
-      <c r="D66" s="161" t="s">
+      <c r="D66" s="160" t="s">
         <v>20</v>
       </c>
-      <c r="E66" s="162" t="s">
+      <c r="E66" s="161" t="s">
         <v>21</v>
       </c>
-      <c r="F66" s="162">
+      <c r="F66" s="161">
         <v>2.0</v>
       </c>
-      <c r="G66" s="160"/>
+      <c r="G66" s="159"/>
       <c r="H66" s="45">
         <f t="shared" ref="H66:H68" si="12">SUM(M66:P66)</f>
         <v>3</v>
       </c>
-      <c r="I66" s="160"/>
-      <c r="J66" s="163" t="s">
+      <c r="I66" s="159"/>
+      <c r="J66" s="81" t="s">
         <v>81</v>
       </c>
       <c r="K66" s="9"/>
       <c r="L66" s="9"/>
-      <c r="M66" s="164">
+      <c r="M66" s="162">
         <v>3.0</v>
       </c>
-      <c r="N66" s="164" t="s">
+      <c r="N66" s="162" t="s">
         <v>82</v>
       </c>
-      <c r="O66" s="164" t="s">
+      <c r="O66" s="162" t="s">
         <v>82</v>
       </c>
-      <c r="P66" s="164" t="s">
+      <c r="P66" s="162" t="s">
         <v>82</v>
       </c>
-      <c r="Q66" s="165">
+      <c r="Q66" s="163">
         <f t="shared" ref="Q66:Q68" si="13">SUM(M66:P66)</f>
         <v>3</v>
       </c>
@@ -5275,16 +5157,16 @@
     <row r="67" ht="16.5" customHeight="1">
       <c r="A67" s="103"/>
       <c r="B67" s="103"/>
-      <c r="C67" s="160" t="s">
+      <c r="C67" s="159" t="s">
         <v>83</v>
       </c>
-      <c r="D67" s="161" t="s">
+      <c r="D67" s="160" t="s">
         <v>20</v>
       </c>
-      <c r="E67" s="166" t="s">
+      <c r="E67" s="164" t="s">
         <v>111</v>
       </c>
-      <c r="F67" s="162">
+      <c r="F67" s="161">
         <v>4.0</v>
       </c>
       <c r="G67" s="103"/>
@@ -5293,24 +5175,24 @@
         <v>3.5</v>
       </c>
       <c r="I67" s="103"/>
-      <c r="J67" s="163" t="s">
+      <c r="J67" s="81" t="s">
         <v>57</v>
       </c>
       <c r="K67" s="9"/>
       <c r="L67" s="9"/>
-      <c r="M67" s="164">
+      <c r="M67" s="162">
         <v>1.0</v>
       </c>
-      <c r="N67" s="164">
+      <c r="N67" s="162">
         <v>1.0</v>
       </c>
-      <c r="O67" s="164">
+      <c r="O67" s="162">
         <v>1.0</v>
       </c>
-      <c r="P67" s="164">
+      <c r="P67" s="162">
         <v>0.5</v>
       </c>
-      <c r="Q67" s="165">
+      <c r="Q67" s="163">
         <f t="shared" si="13"/>
         <v>3.5</v>
       </c>
@@ -5333,16 +5215,16 @@
     <row r="68" ht="16.5" customHeight="1">
       <c r="A68" s="103"/>
       <c r="B68" s="103"/>
-      <c r="C68" s="167" t="s">
+      <c r="C68" s="165" t="s">
         <v>88</v>
       </c>
-      <c r="D68" s="161" t="s">
+      <c r="D68" s="160" t="s">
         <v>52</v>
       </c>
-      <c r="E68" s="168" t="s">
+      <c r="E68" s="166" t="s">
         <v>61</v>
       </c>
-      <c r="F68" s="162">
+      <c r="F68" s="161">
         <v>4.0</v>
       </c>
       <c r="G68" s="103"/>
@@ -5351,24 +5233,24 @@
         <v>1.5</v>
       </c>
       <c r="I68" s="103"/>
-      <c r="J68" s="163" t="s">
+      <c r="J68" s="81" t="s">
         <v>57</v>
       </c>
       <c r="K68" s="9"/>
       <c r="L68" s="9"/>
-      <c r="M68" s="164" t="s">
+      <c r="M68" s="162" t="s">
         <v>82</v>
       </c>
-      <c r="N68" s="164">
+      <c r="N68" s="162">
         <v>1.5</v>
       </c>
-      <c r="O68" s="164" t="s">
+      <c r="O68" s="162" t="s">
         <v>82</v>
       </c>
-      <c r="P68" s="164" t="s">
+      <c r="P68" s="162" t="s">
         <v>82</v>
       </c>
-      <c r="Q68" s="165">
+      <c r="Q68" s="163">
         <f t="shared" si="13"/>
         <v>1.5</v>
       </c>
@@ -5392,7 +5274,7 @@
     </row>
     <row r="69">
       <c r="A69" s="103"/>
-      <c r="B69" s="158" t="s">
+      <c r="B69" s="157" t="s">
         <v>50</v>
       </c>
       <c r="C69" s="69"/>
@@ -5433,7 +5315,7 @@
       <c r="AF69" s="5"/>
     </row>
     <row r="70">
-      <c r="A70" s="157"/>
+      <c r="A70" s="156"/>
       <c r="B70" s="103"/>
       <c r="C70" s="40" t="s">
         <v>89</v>
@@ -5453,24 +5335,24 @@
         <v>4</v>
       </c>
       <c r="I70" s="103"/>
-      <c r="J70" s="163" t="s">
+      <c r="J70" s="81" t="s">
         <v>57</v>
       </c>
       <c r="K70" s="5"/>
       <c r="L70" s="5"/>
-      <c r="M70" s="164">
+      <c r="M70" s="162">
         <v>1.5</v>
       </c>
-      <c r="N70" s="164">
+      <c r="N70" s="162">
         <v>1.5</v>
       </c>
-      <c r="O70" s="164">
+      <c r="O70" s="162">
         <v>1.0</v>
       </c>
-      <c r="P70" s="164" t="s">
+      <c r="P70" s="162" t="s">
         <v>82</v>
       </c>
-      <c r="Q70" s="165">
+      <c r="Q70" s="163">
         <f t="shared" ref="Q70:Q77" si="15">SUM(M70:P70)</f>
         <v>4</v>
       </c>
@@ -5491,7 +5373,7 @@
       <c r="AF70" s="5"/>
     </row>
     <row r="71">
-      <c r="A71" s="157"/>
+      <c r="A71" s="156"/>
       <c r="B71" s="103"/>
       <c r="C71" s="112" t="s">
         <v>102</v>
@@ -5511,24 +5393,24 @@
         <v>3</v>
       </c>
       <c r="I71" s="103"/>
-      <c r="J71" s="163" t="s">
+      <c r="J71" s="81" t="s">
         <v>54</v>
       </c>
       <c r="K71" s="5"/>
       <c r="L71" s="5"/>
-      <c r="M71" s="164">
+      <c r="M71" s="162">
         <v>2.0</v>
       </c>
-      <c r="N71" s="164">
+      <c r="N71" s="162">
         <v>1.0</v>
       </c>
-      <c r="O71" s="164" t="s">
+      <c r="O71" s="162" t="s">
         <v>82</v>
       </c>
-      <c r="P71" s="164" t="s">
+      <c r="P71" s="162" t="s">
         <v>82</v>
       </c>
-      <c r="Q71" s="165">
+      <c r="Q71" s="163">
         <f t="shared" si="15"/>
         <v>3</v>
       </c>
@@ -5551,8 +5433,8 @@
       <c r="AF71" s="5"/>
     </row>
     <row r="72">
-      <c r="A72" s="157"/>
-      <c r="B72" s="157"/>
+      <c r="A72" s="156"/>
+      <c r="B72" s="156"/>
       <c r="C72" s="112" t="s">
         <v>104</v>
       </c>
@@ -5571,24 +5453,24 @@
         <v>0</v>
       </c>
       <c r="I72" s="103"/>
-      <c r="J72" s="163" t="s">
+      <c r="J72" s="81" t="s">
         <v>54</v>
       </c>
       <c r="K72" s="5"/>
       <c r="L72" s="5"/>
-      <c r="M72" s="164" t="s">
+      <c r="M72" s="162" t="s">
         <v>82</v>
       </c>
-      <c r="N72" s="164" t="s">
+      <c r="N72" s="162" t="s">
         <v>82</v>
       </c>
-      <c r="O72" s="164" t="s">
+      <c r="O72" s="162" t="s">
         <v>82</v>
       </c>
-      <c r="P72" s="164" t="s">
+      <c r="P72" s="162" t="s">
         <v>82</v>
       </c>
-      <c r="Q72" s="165">
+      <c r="Q72" s="163">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -5611,8 +5493,8 @@
       <c r="AF72" s="5"/>
     </row>
     <row r="73">
-      <c r="A73" s="157"/>
-      <c r="B73" s="157"/>
+      <c r="A73" s="156"/>
+      <c r="B73" s="156"/>
       <c r="C73" s="112" t="s">
         <v>105</v>
       </c>
@@ -5630,25 +5512,25 @@
         <f t="shared" si="14"/>
         <v>1.6</v>
       </c>
-      <c r="I73" s="169"/>
-      <c r="J73" s="163" t="s">
+      <c r="I73" s="156"/>
+      <c r="J73" s="81" t="s">
         <v>81</v>
       </c>
       <c r="K73" s="5"/>
       <c r="L73" s="5"/>
-      <c r="M73" s="164">
+      <c r="M73" s="162">
         <v>0.6</v>
       </c>
-      <c r="N73" s="164">
+      <c r="N73" s="162">
         <v>1.0</v>
       </c>
-      <c r="O73" s="164" t="s">
+      <c r="O73" s="162" t="s">
         <v>82</v>
       </c>
-      <c r="P73" s="164" t="s">
+      <c r="P73" s="162" t="s">
         <v>82</v>
       </c>
-      <c r="Q73" s="165">
+      <c r="Q73" s="163">
         <f t="shared" si="15"/>
         <v>1.6</v>
       </c>
@@ -5672,7 +5554,7 @@
     </row>
     <row r="74">
       <c r="A74" s="103"/>
-      <c r="B74" s="157"/>
+      <c r="B74" s="156"/>
       <c r="C74" s="50" t="s">
         <v>69</v>
       </c>
@@ -5690,25 +5572,25 @@
         <f t="shared" si="14"/>
         <v>0.2</v>
       </c>
-      <c r="I74" s="169"/>
-      <c r="J74" s="163" t="s">
+      <c r="I74" s="156"/>
+      <c r="J74" s="81" t="s">
         <v>57</v>
       </c>
       <c r="K74" s="5"/>
       <c r="L74" s="5"/>
-      <c r="M74" s="164">
+      <c r="M74" s="162">
         <v>0.2</v>
       </c>
-      <c r="N74" s="164" t="s">
+      <c r="N74" s="162" t="s">
         <v>82</v>
       </c>
-      <c r="O74" s="164" t="s">
+      <c r="O74" s="162" t="s">
         <v>82</v>
       </c>
-      <c r="P74" s="164" t="s">
+      <c r="P74" s="162" t="s">
         <v>82</v>
       </c>
-      <c r="Q74" s="165">
+      <c r="Q74" s="163">
         <f t="shared" si="15"/>
         <v>0.2</v>
       </c>
@@ -5730,11 +5612,11 @@
     </row>
     <row r="75">
       <c r="A75" s="103"/>
-      <c r="B75" s="157"/>
+      <c r="B75" s="156"/>
       <c r="C75" s="114" t="s">
         <v>114</v>
       </c>
-      <c r="D75" s="170" t="s">
+      <c r="D75" s="167" t="s">
         <v>52</v>
       </c>
       <c r="E75" s="52" t="s">
@@ -5748,25 +5630,25 @@
         <f t="shared" si="14"/>
         <v>4</v>
       </c>
-      <c r="I75" s="169"/>
-      <c r="J75" s="163" t="s">
+      <c r="I75" s="156"/>
+      <c r="J75" s="81" t="s">
         <v>81</v>
       </c>
       <c r="K75" s="5"/>
       <c r="L75" s="5"/>
-      <c r="M75" s="164">
+      <c r="M75" s="162">
         <v>1.5</v>
       </c>
-      <c r="N75" s="164">
+      <c r="N75" s="162">
         <v>1.5</v>
       </c>
-      <c r="O75" s="164" t="s">
+      <c r="O75" s="162" t="s">
         <v>82</v>
       </c>
-      <c r="P75" s="164">
+      <c r="P75" s="162">
         <v>1.0</v>
       </c>
-      <c r="Q75" s="165">
+      <c r="Q75" s="163">
         <f t="shared" si="15"/>
         <v>4</v>
       </c>
@@ -5788,11 +5670,11 @@
     </row>
     <row r="76">
       <c r="A76" s="103"/>
-      <c r="B76" s="157"/>
+      <c r="B76" s="156"/>
       <c r="C76" s="114" t="s">
         <v>88</v>
       </c>
-      <c r="D76" s="170" t="s">
+      <c r="D76" s="167" t="s">
         <v>52</v>
       </c>
       <c r="E76" s="52" t="s">
@@ -5807,24 +5689,24 @@
         <v>1.3</v>
       </c>
       <c r="I76" s="103"/>
-      <c r="J76" s="163" t="s">
+      <c r="J76" s="81" t="s">
         <v>57</v>
       </c>
       <c r="K76" s="5"/>
       <c r="L76" s="5"/>
-      <c r="M76" s="164">
+      <c r="M76" s="162">
         <v>0.3</v>
       </c>
-      <c r="N76" s="164">
+      <c r="N76" s="162">
         <v>1.0</v>
       </c>
-      <c r="O76" s="164" t="s">
+      <c r="O76" s="162" t="s">
         <v>82</v>
       </c>
-      <c r="P76" s="164" t="s">
+      <c r="P76" s="162" t="s">
         <v>82</v>
       </c>
-      <c r="Q76" s="171">
+      <c r="Q76" s="162">
         <f t="shared" si="15"/>
         <v>1.3</v>
       </c>
@@ -5848,7 +5730,7 @@
     </row>
     <row r="77">
       <c r="A77" s="103"/>
-      <c r="B77" s="157"/>
+      <c r="B77" s="156"/>
       <c r="C77" s="114" t="s">
         <v>115</v>
       </c>
@@ -5867,24 +5749,24 @@
         <v>1.2</v>
       </c>
       <c r="I77" s="103"/>
-      <c r="J77" s="163" t="s">
+      <c r="J77" s="81" t="s">
         <v>81</v>
       </c>
       <c r="K77" s="5"/>
       <c r="L77" s="5"/>
-      <c r="M77" s="164">
+      <c r="M77" s="162">
         <v>0.4</v>
       </c>
-      <c r="N77" s="164">
+      <c r="N77" s="162">
         <v>0.4</v>
       </c>
-      <c r="O77" s="164">
+      <c r="O77" s="162">
         <v>0.4</v>
       </c>
-      <c r="P77" s="164" t="s">
+      <c r="P77" s="162" t="s">
         <v>82</v>
       </c>
-      <c r="Q77" s="165">
+      <c r="Q77" s="163">
         <f t="shared" si="15"/>
         <v>1.2</v>
       </c>
@@ -5906,7 +5788,7 @@
     </row>
     <row r="78">
       <c r="A78" s="103"/>
-      <c r="B78" s="158" t="s">
+      <c r="B78" s="157" t="s">
         <v>71</v>
       </c>
       <c r="C78" s="69"/>
@@ -5947,44 +5829,44 @@
       <c r="AF78" s="5"/>
     </row>
     <row r="79">
-      <c r="A79" s="160"/>
-      <c r="B79" s="160"/>
-      <c r="C79" s="172" t="s">
+      <c r="A79" s="159"/>
+      <c r="B79" s="159"/>
+      <c r="C79" s="168" t="s">
         <v>106</v>
       </c>
-      <c r="D79" s="173" t="s">
+      <c r="D79" s="169" t="s">
         <v>107</v>
       </c>
-      <c r="E79" s="174" t="s">
+      <c r="E79" s="170" t="s">
         <v>117</v>
       </c>
-      <c r="F79" s="175">
+      <c r="F79" s="171">
         <v>2.0</v>
       </c>
-      <c r="G79" s="160"/>
+      <c r="G79" s="159"/>
       <c r="H79" s="45">
         <f t="shared" ref="H79:H81" si="16">SUM(M79:P79)</f>
         <v>1</v>
       </c>
-      <c r="I79" s="160"/>
+      <c r="I79" s="159"/>
       <c r="J79" s="81" t="s">
         <v>67</v>
       </c>
       <c r="K79" s="5"/>
       <c r="L79" s="5"/>
-      <c r="M79" s="164">
+      <c r="M79" s="162">
         <v>0.5</v>
       </c>
-      <c r="N79" s="164">
+      <c r="N79" s="162">
         <v>0.5</v>
       </c>
-      <c r="O79" s="164" t="s">
+      <c r="O79" s="162" t="s">
         <v>82</v>
       </c>
-      <c r="P79" s="164" t="s">
+      <c r="P79" s="162" t="s">
         <v>82</v>
       </c>
-      <c r="Q79" s="165">
+      <c r="Q79" s="163">
         <f t="shared" ref="Q79:Q96" si="17">SUM(M79:P79)</f>
         <v>1</v>
       </c>
@@ -6005,44 +5887,44 @@
       <c r="AF79" s="5"/>
     </row>
     <row r="80">
-      <c r="A80" s="176"/>
-      <c r="B80" s="176"/>
+      <c r="A80" s="172"/>
+      <c r="B80" s="172"/>
       <c r="C80" s="50" t="s">
         <v>96</v>
       </c>
       <c r="D80" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="E80" s="177" t="s">
+      <c r="E80" s="173" t="s">
         <v>118</v>
       </c>
       <c r="F80" s="115">
         <v>2.0</v>
       </c>
-      <c r="G80" s="176"/>
+      <c r="G80" s="172"/>
       <c r="H80" s="45">
         <f t="shared" si="16"/>
         <v>0.4</v>
       </c>
-      <c r="I80" s="176"/>
-      <c r="J80" s="163" t="s">
+      <c r="I80" s="172"/>
+      <c r="J80" s="81" t="s">
         <v>57</v>
       </c>
       <c r="K80" s="5"/>
       <c r="L80" s="5"/>
-      <c r="M80" s="164">
+      <c r="M80" s="162">
         <v>0.2</v>
       </c>
-      <c r="N80" s="164">
+      <c r="N80" s="162">
         <v>0.2</v>
       </c>
-      <c r="O80" s="164" t="s">
+      <c r="O80" s="162" t="s">
         <v>82</v>
       </c>
-      <c r="P80" s="164" t="s">
+      <c r="P80" s="162" t="s">
         <v>82</v>
       </c>
-      <c r="Q80" s="165">
+      <c r="Q80" s="163">
         <f t="shared" si="17"/>
         <v>0.4</v>
       </c>
@@ -6071,7 +5953,7 @@
       <c r="D81" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="E81" s="177" t="s">
+      <c r="E81" s="173" t="s">
         <v>120</v>
       </c>
       <c r="F81" s="115">
@@ -6083,24 +5965,24 @@
         <v>1.7</v>
       </c>
       <c r="I81" s="103"/>
-      <c r="J81" s="163" t="s">
+      <c r="J81" s="81" t="s">
         <v>57</v>
       </c>
       <c r="K81" s="5"/>
       <c r="L81" s="5"/>
-      <c r="M81" s="164">
+      <c r="M81" s="162">
         <v>0.5</v>
       </c>
-      <c r="N81" s="164">
+      <c r="N81" s="162">
         <v>0.5</v>
       </c>
-      <c r="O81" s="164">
+      <c r="O81" s="162">
         <v>0.5</v>
       </c>
-      <c r="P81" s="164">
+      <c r="P81" s="162">
         <v>0.2</v>
       </c>
-      <c r="Q81" s="165">
+      <c r="Q81" s="163">
         <f t="shared" si="17"/>
         <v>1.7</v>
       </c>
@@ -6121,7 +6003,7 @@
       <c r="AF81" s="5"/>
     </row>
     <row r="82">
-      <c r="A82" s="178" t="s">
+      <c r="A82" s="174" t="s">
         <v>121</v>
       </c>
       <c r="B82" s="32" t="s">
@@ -6138,7 +6020,7 @@
       <c r="H82" s="71"/>
       <c r="I82" s="106">
         <f>SUM(H83:H86)</f>
-        <v>1</v>
+        <v>11.7</v>
       </c>
       <c r="J82" s="6"/>
       <c r="K82" s="6"/>
@@ -6168,37 +6050,43 @@
       <c r="AF82" s="5"/>
     </row>
     <row r="83">
-      <c r="A83" s="179"/>
-      <c r="B83" s="180"/>
-      <c r="C83" s="181" t="s">
+      <c r="A83" s="123"/>
+      <c r="B83" s="124"/>
+      <c r="C83" s="59" t="s">
         <v>80</v>
       </c>
       <c r="D83" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="E83" s="182" t="s">
+      <c r="E83" s="125" t="s">
         <v>21</v>
       </c>
-      <c r="F83" s="183">
+      <c r="F83" s="126">
         <v>2.0</v>
       </c>
-      <c r="G83" s="184"/>
+      <c r="G83" s="127"/>
       <c r="H83" s="64">
         <f t="shared" ref="H83:H86" si="18">SUM(M83:P83)</f>
         <v>0.5</v>
       </c>
-      <c r="I83" s="185"/>
-      <c r="J83" s="163" t="s">
-        <v>54</v>
-      </c>
-      <c r="K83" s="186"/>
-      <c r="L83" s="186"/>
-      <c r="M83" s="187">
+      <c r="I83" s="128"/>
+      <c r="J83" s="175" t="s">
+        <v>81</v>
+      </c>
+      <c r="K83" s="5"/>
+      <c r="L83" s="5"/>
+      <c r="M83" s="129">
         <v>0.5</v>
       </c>
-      <c r="N83" s="188"/>
-      <c r="O83" s="188"/>
-      <c r="P83" s="188"/>
+      <c r="N83" s="176" t="s">
+        <v>82</v>
+      </c>
+      <c r="O83" s="176" t="s">
+        <v>82</v>
+      </c>
+      <c r="P83" s="176" t="s">
+        <v>82</v>
+      </c>
       <c r="Q83" s="130">
         <f t="shared" si="17"/>
         <v>0.5</v>
@@ -6220,9 +6108,9 @@
       <c r="AF83" s="5"/>
     </row>
     <row r="84">
-      <c r="A84" s="189"/>
-      <c r="B84" s="190"/>
-      <c r="C84" s="191" t="s">
+      <c r="A84" s="67"/>
+      <c r="B84" s="86"/>
+      <c r="C84" s="131" t="s">
         <v>83</v>
       </c>
       <c r="D84" s="75" t="s">
@@ -6231,28 +6119,32 @@
       <c r="E84" s="132" t="s">
         <v>122</v>
       </c>
-      <c r="F84" s="192">
+      <c r="F84" s="133">
         <v>1.0</v>
       </c>
-      <c r="G84" s="193"/>
+      <c r="G84" s="78"/>
       <c r="H84" s="134">
         <f t="shared" si="18"/>
         <v>0.5</v>
       </c>
-      <c r="I84" s="193"/>
-      <c r="J84" s="163" t="s">
-        <v>54</v>
-      </c>
-      <c r="K84" s="186"/>
-      <c r="L84" s="186"/>
-      <c r="M84" s="135">
+      <c r="I84" s="78"/>
+      <c r="J84" s="175" t="s">
+        <v>57</v>
+      </c>
+      <c r="K84" s="5"/>
+      <c r="L84" s="5"/>
+      <c r="M84" s="100">
         <v>0.25</v>
       </c>
-      <c r="N84" s="135">
+      <c r="N84" s="100">
         <v>0.25</v>
       </c>
-      <c r="O84" s="135"/>
-      <c r="P84" s="135"/>
+      <c r="O84" s="177" t="s">
+        <v>82</v>
+      </c>
+      <c r="P84" s="177" t="s">
+        <v>82</v>
+      </c>
       <c r="Q84" s="101">
         <f t="shared" si="17"/>
         <v>0.5</v>
@@ -6274,38 +6166,46 @@
       <c r="AF84" s="5"/>
     </row>
     <row r="85">
-      <c r="A85" s="189"/>
-      <c r="B85" s="190"/>
-      <c r="C85" s="194" t="s">
+      <c r="A85" s="67"/>
+      <c r="B85" s="86"/>
+      <c r="C85" s="85" t="s">
         <v>123</v>
       </c>
       <c r="D85" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="E85" s="195" t="s">
+      <c r="E85" s="132" t="s">
         <v>61</v>
       </c>
-      <c r="F85" s="192">
+      <c r="F85" s="133">
         <v>1.0</v>
       </c>
-      <c r="G85" s="193"/>
+      <c r="G85" s="78"/>
       <c r="H85" s="134">
         <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="I85" s="193"/>
-      <c r="J85" s="163" t="s">
-        <v>67</v>
-      </c>
-      <c r="K85" s="186"/>
-      <c r="L85" s="186"/>
-      <c r="M85" s="135"/>
-      <c r="N85" s="135"/>
-      <c r="O85" s="135"/>
-      <c r="P85" s="135"/>
+        <v>5</v>
+      </c>
+      <c r="I85" s="78"/>
+      <c r="J85" s="175" t="s">
+        <v>81</v>
+      </c>
+      <c r="K85" s="5"/>
+      <c r="L85" s="5"/>
+      <c r="M85" s="177">
+        <v>5.0</v>
+      </c>
+      <c r="N85" s="177" t="s">
+        <v>82</v>
+      </c>
+      <c r="O85" s="177" t="s">
+        <v>82</v>
+      </c>
+      <c r="P85" s="177" t="s">
+        <v>82</v>
+      </c>
       <c r="Q85" s="101">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R85" s="5"/>
       <c r="S85" s="5"/>
@@ -6324,38 +6224,46 @@
       <c r="AF85" s="5"/>
     </row>
     <row r="86">
-      <c r="A86" s="189"/>
-      <c r="B86" s="196"/>
-      <c r="C86" s="197" t="s">
+      <c r="A86" s="67"/>
+      <c r="B86" s="87"/>
+      <c r="C86" s="136" t="s">
         <v>124</v>
       </c>
       <c r="D86" s="89" t="s">
         <v>52</v>
       </c>
-      <c r="E86" s="198" t="s">
+      <c r="E86" s="137" t="s">
         <v>64</v>
       </c>
-      <c r="F86" s="199">
+      <c r="F86" s="138">
         <v>1.5</v>
       </c>
-      <c r="G86" s="200"/>
-      <c r="H86" s="140">
+      <c r="G86" s="92"/>
+      <c r="H86" s="139">
         <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="I86" s="200"/>
-      <c r="J86" s="163" t="s">
-        <v>67</v>
-      </c>
-      <c r="K86" s="186"/>
-      <c r="L86" s="186"/>
-      <c r="M86" s="201"/>
-      <c r="N86" s="201"/>
-      <c r="O86" s="202"/>
-      <c r="P86" s="202"/>
-      <c r="Q86" s="142">
+        <v>5.7</v>
+      </c>
+      <c r="I86" s="92"/>
+      <c r="J86" s="175" t="s">
+        <v>81</v>
+      </c>
+      <c r="K86" s="5"/>
+      <c r="L86" s="5"/>
+      <c r="M86" s="178">
+        <v>4.2</v>
+      </c>
+      <c r="N86" s="140">
+        <v>1.5</v>
+      </c>
+      <c r="O86" s="178" t="s">
+        <v>82</v>
+      </c>
+      <c r="P86" s="178" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q86" s="141">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>5.7</v>
       </c>
       <c r="R86" s="5"/>
       <c r="S86" s="5"/>
@@ -6374,30 +6282,30 @@
       <c r="AF86" s="5"/>
     </row>
     <row r="87">
-      <c r="A87" s="189"/>
-      <c r="B87" s="203" t="s">
+      <c r="A87" s="67"/>
+      <c r="B87" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="C87" s="204"/>
+      <c r="C87" s="104"/>
       <c r="D87" s="69"/>
-      <c r="E87" s="205"/>
+      <c r="E87" s="70"/>
       <c r="F87" s="98"/>
       <c r="G87" s="105">
         <f>SUM(F88:F92)</f>
         <v>6.5</v>
       </c>
       <c r="H87" s="98"/>
-      <c r="I87" s="106">
+      <c r="I87" s="105">
         <f>SUM(H88:H92)</f>
-        <v>0</v>
-      </c>
-      <c r="J87" s="163"/>
-      <c r="K87" s="186"/>
-      <c r="L87" s="186"/>
-      <c r="M87" s="206"/>
-      <c r="N87" s="206"/>
-      <c r="O87" s="206"/>
-      <c r="P87" s="206"/>
+        <v>6.3</v>
+      </c>
+      <c r="J87" s="81"/>
+      <c r="K87" s="5"/>
+      <c r="L87" s="5"/>
+      <c r="M87" s="107"/>
+      <c r="N87" s="107"/>
+      <c r="O87" s="107"/>
+      <c r="P87" s="107"/>
       <c r="Q87" s="107">
         <f t="shared" si="17"/>
         <v>0</v>
@@ -6419,38 +6327,45 @@
       <c r="AF87" s="5"/>
     </row>
     <row r="88">
-      <c r="A88" s="189"/>
-      <c r="B88" s="190"/>
-      <c r="C88" s="191" t="s">
+      <c r="A88" s="67"/>
+      <c r="B88" s="86"/>
+      <c r="C88" s="131" t="s">
         <v>89</v>
       </c>
       <c r="D88" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="E88" s="195" t="s">
+      <c r="E88" s="132" t="s">
         <v>64</v>
       </c>
-      <c r="F88" s="192">
+      <c r="F88" s="133">
         <v>1.0</v>
       </c>
-      <c r="G88" s="193"/>
-      <c r="H88" s="134">
-        <f t="shared" ref="H88:H92" si="19">SUM(M88:P88)</f>
-        <v>0</v>
-      </c>
-      <c r="I88" s="193"/>
-      <c r="J88" s="163" t="s">
-        <v>67</v>
-      </c>
-      <c r="K88" s="186"/>
-      <c r="L88" s="186"/>
-      <c r="M88" s="207"/>
-      <c r="N88" s="135"/>
-      <c r="O88" s="207"/>
-      <c r="P88" s="207"/>
+      <c r="G88" s="78"/>
+      <c r="H88" s="133">
+        <v>1.0</v>
+      </c>
+      <c r="I88" s="78"/>
+      <c r="J88" s="81" t="s">
+        <v>57</v>
+      </c>
+      <c r="K88" s="5"/>
+      <c r="L88" s="5"/>
+      <c r="M88" s="177">
+        <v>2.0</v>
+      </c>
+      <c r="N88" s="100">
+        <v>1.0</v>
+      </c>
+      <c r="O88" s="177" t="s">
+        <v>82</v>
+      </c>
+      <c r="P88" s="177" t="s">
+        <v>82</v>
+      </c>
       <c r="Q88" s="101">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R88" s="5"/>
       <c r="S88" s="5"/>
@@ -6469,9 +6384,9 @@
       <c r="AF88" s="5"/>
     </row>
     <row r="89">
-      <c r="A89" s="189"/>
-      <c r="B89" s="190"/>
-      <c r="C89" s="194" t="s">
+      <c r="A89" s="67"/>
+      <c r="B89" s="86"/>
+      <c r="C89" s="85" t="s">
         <v>125</v>
       </c>
       <c r="D89" s="75" t="s">
@@ -6480,27 +6395,35 @@
       <c r="E89" s="132" t="s">
         <v>126</v>
       </c>
-      <c r="F89" s="192">
+      <c r="F89" s="133">
         <v>2.0</v>
       </c>
-      <c r="G89" s="193"/>
+      <c r="G89" s="78"/>
       <c r="H89" s="134">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="I89" s="193"/>
-      <c r="J89" s="163" t="s">
-        <v>67</v>
-      </c>
-      <c r="K89" s="186"/>
-      <c r="L89" s="186"/>
-      <c r="M89" s="135"/>
-      <c r="N89" s="207"/>
-      <c r="O89" s="207"/>
-      <c r="P89" s="135"/>
+        <f t="shared" ref="H89:H92" si="19">SUM(M89:P89)</f>
+        <v>3</v>
+      </c>
+      <c r="I89" s="78"/>
+      <c r="J89" s="175" t="s">
+        <v>76</v>
+      </c>
+      <c r="K89" s="5"/>
+      <c r="L89" s="5"/>
+      <c r="M89" s="177">
+        <v>2.0</v>
+      </c>
+      <c r="N89" s="100">
+        <v>1.0</v>
+      </c>
+      <c r="O89" s="177" t="s">
+        <v>82</v>
+      </c>
+      <c r="P89" s="177" t="s">
+        <v>82</v>
+      </c>
       <c r="Q89" s="101">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R89" s="5"/>
       <c r="S89" s="5"/>
@@ -6519,38 +6442,46 @@
       <c r="AF89" s="5"/>
     </row>
     <row r="90">
-      <c r="A90" s="189"/>
-      <c r="B90" s="190"/>
-      <c r="C90" s="194" t="s">
+      <c r="A90" s="67"/>
+      <c r="B90" s="86"/>
+      <c r="C90" s="85" t="s">
         <v>127</v>
       </c>
       <c r="D90" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="E90" s="195" t="s">
+      <c r="E90" s="132" t="s">
         <v>66</v>
       </c>
-      <c r="F90" s="192">
+      <c r="F90" s="133">
         <v>1.0</v>
       </c>
-      <c r="G90" s="193"/>
+      <c r="G90" s="78"/>
       <c r="H90" s="134">
         <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="I90" s="193"/>
-      <c r="J90" s="163" t="s">
-        <v>67</v>
-      </c>
-      <c r="K90" s="186"/>
-      <c r="L90" s="186"/>
-      <c r="M90" s="207"/>
-      <c r="N90" s="207"/>
-      <c r="O90" s="207"/>
-      <c r="P90" s="135"/>
+        <v>1</v>
+      </c>
+      <c r="I90" s="78"/>
+      <c r="J90" s="175" t="s">
+        <v>81</v>
+      </c>
+      <c r="K90" s="5"/>
+      <c r="L90" s="5"/>
+      <c r="M90" s="177">
+        <v>1.0</v>
+      </c>
+      <c r="N90" s="177" t="s">
+        <v>82</v>
+      </c>
+      <c r="O90" s="177" t="s">
+        <v>82</v>
+      </c>
+      <c r="P90" s="177" t="s">
+        <v>82</v>
+      </c>
       <c r="Q90" s="101">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R90" s="5"/>
       <c r="S90" s="5"/>
@@ -6569,38 +6500,46 @@
       <c r="AF90" s="5"/>
     </row>
     <row r="91">
-      <c r="A91" s="189"/>
-      <c r="B91" s="190"/>
-      <c r="C91" s="194" t="s">
+      <c r="A91" s="67"/>
+      <c r="B91" s="86"/>
+      <c r="C91" s="85" t="s">
         <v>128</v>
       </c>
       <c r="D91" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="E91" s="195" t="s">
+      <c r="E91" s="132" t="s">
         <v>61</v>
       </c>
-      <c r="F91" s="192">
+      <c r="F91" s="133">
         <v>1.5</v>
       </c>
-      <c r="G91" s="193"/>
+      <c r="G91" s="78"/>
       <c r="H91" s="134">
         <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="I91" s="193"/>
-      <c r="J91" s="163" t="s">
-        <v>67</v>
-      </c>
-      <c r="K91" s="186"/>
-      <c r="L91" s="186"/>
-      <c r="M91" s="207"/>
-      <c r="N91" s="207"/>
-      <c r="O91" s="207"/>
-      <c r="P91" s="135"/>
+        <v>1</v>
+      </c>
+      <c r="I91" s="78"/>
+      <c r="J91" s="175" t="s">
+        <v>76</v>
+      </c>
+      <c r="K91" s="5"/>
+      <c r="L91" s="5"/>
+      <c r="M91" s="177">
+        <v>1.0</v>
+      </c>
+      <c r="N91" s="177" t="s">
+        <v>82</v>
+      </c>
+      <c r="O91" s="177" t="s">
+        <v>82</v>
+      </c>
+      <c r="P91" s="177" t="s">
+        <v>82</v>
+      </c>
       <c r="Q91" s="101">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R91" s="5"/>
       <c r="S91" s="5"/>
@@ -6619,38 +6558,46 @@
       <c r="AF91" s="5"/>
     </row>
     <row r="92">
-      <c r="A92" s="189"/>
-      <c r="B92" s="196"/>
-      <c r="C92" s="208" t="s">
+      <c r="A92" s="67"/>
+      <c r="B92" s="87"/>
+      <c r="C92" s="142" t="s">
         <v>69</v>
       </c>
       <c r="D92" s="89" t="s">
         <v>52</v>
       </c>
-      <c r="E92" s="138" t="s">
+      <c r="E92" s="137" t="s">
         <v>129</v>
       </c>
-      <c r="F92" s="199">
+      <c r="F92" s="138">
         <v>1.0</v>
       </c>
-      <c r="G92" s="200"/>
-      <c r="H92" s="140">
+      <c r="G92" s="92"/>
+      <c r="H92" s="139">
         <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="I92" s="200"/>
-      <c r="J92" s="163" t="s">
-        <v>67</v>
-      </c>
-      <c r="K92" s="186"/>
-      <c r="L92" s="186"/>
-      <c r="M92" s="202"/>
-      <c r="N92" s="202"/>
-      <c r="O92" s="202"/>
-      <c r="P92" s="202"/>
-      <c r="Q92" s="142">
+        <v>0.3</v>
+      </c>
+      <c r="I92" s="92"/>
+      <c r="J92" s="175" t="s">
+        <v>54</v>
+      </c>
+      <c r="K92" s="5"/>
+      <c r="L92" s="5"/>
+      <c r="M92" s="178">
+        <v>0.3</v>
+      </c>
+      <c r="N92" s="178" t="s">
+        <v>82</v>
+      </c>
+      <c r="O92" s="178" t="s">
+        <v>82</v>
+      </c>
+      <c r="P92" s="178" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q92" s="141">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="R92" s="5"/>
       <c r="S92" s="5"/>
@@ -6669,31 +6616,31 @@
       <c r="AF92" s="5"/>
     </row>
     <row r="93">
-      <c r="A93" s="189"/>
-      <c r="B93" s="209" t="s">
+      <c r="A93" s="67"/>
+      <c r="B93" s="143" t="s">
         <v>71</v>
       </c>
-      <c r="C93" s="210"/>
-      <c r="D93" s="146"/>
-      <c r="E93" s="211"/>
-      <c r="F93" s="148"/>
-      <c r="G93" s="149">
+      <c r="C93" s="144"/>
+      <c r="D93" s="145"/>
+      <c r="E93" s="146"/>
+      <c r="F93" s="147"/>
+      <c r="G93" s="148">
         <f>SUM(F94:F95)</f>
         <v>7</v>
       </c>
-      <c r="H93" s="148"/>
-      <c r="I93" s="150">
+      <c r="H93" s="147"/>
+      <c r="I93" s="149">
         <f>SUM(H94:H95)</f>
-        <v>0</v>
-      </c>
-      <c r="J93" s="163"/>
-      <c r="K93" s="186"/>
-      <c r="L93" s="186"/>
-      <c r="M93" s="212"/>
-      <c r="N93" s="212"/>
-      <c r="O93" s="212"/>
-      <c r="P93" s="212"/>
-      <c r="Q93" s="151">
+        <v>3.2</v>
+      </c>
+      <c r="J93" s="81"/>
+      <c r="K93" s="5"/>
+      <c r="L93" s="5"/>
+      <c r="M93" s="150"/>
+      <c r="N93" s="150"/>
+      <c r="O93" s="150"/>
+      <c r="P93" s="150"/>
+      <c r="Q93" s="150">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
@@ -6714,38 +6661,46 @@
       <c r="AF93" s="5"/>
     </row>
     <row r="94">
-      <c r="A94" s="179"/>
-      <c r="B94" s="180"/>
-      <c r="C94" s="213" t="s">
+      <c r="A94" s="123"/>
+      <c r="B94" s="124"/>
+      <c r="C94" s="179" t="s">
         <v>130</v>
       </c>
       <c r="D94" s="60" t="s">
         <v>107</v>
       </c>
-      <c r="E94" s="152" t="s">
+      <c r="E94" s="151" t="s">
         <v>131</v>
       </c>
-      <c r="F94" s="153">
+      <c r="F94" s="152">
         <v>6.0</v>
       </c>
-      <c r="G94" s="184"/>
-      <c r="H94" s="154">
+      <c r="G94" s="127"/>
+      <c r="H94" s="153">
         <f t="shared" ref="H94:H96" si="20">SUM(M94:P94)</f>
-        <v>0</v>
-      </c>
-      <c r="I94" s="185"/>
-      <c r="J94" s="163" t="s">
-        <v>67</v>
-      </c>
-      <c r="K94" s="186"/>
-      <c r="L94" s="186"/>
-      <c r="M94" s="187"/>
-      <c r="N94" s="187"/>
-      <c r="O94" s="188"/>
-      <c r="P94" s="188"/>
+        <v>2</v>
+      </c>
+      <c r="I94" s="128"/>
+      <c r="J94" s="81" t="s">
+        <v>54</v>
+      </c>
+      <c r="K94" s="5"/>
+      <c r="L94" s="5"/>
+      <c r="M94" s="176">
+        <v>1.0</v>
+      </c>
+      <c r="N94" s="129">
+        <v>1.0</v>
+      </c>
+      <c r="O94" s="176" t="s">
+        <v>82</v>
+      </c>
+      <c r="P94" s="176" t="s">
+        <v>82</v>
+      </c>
       <c r="Q94" s="130">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R94" s="5"/>
       <c r="S94" s="5"/>
@@ -6764,38 +6719,46 @@
       <c r="AF94" s="5"/>
     </row>
     <row r="95">
-      <c r="A95" s="214"/>
-      <c r="B95" s="196"/>
-      <c r="C95" s="208" t="s">
+      <c r="A95" s="154"/>
+      <c r="B95" s="87"/>
+      <c r="C95" s="142" t="s">
         <v>96</v>
       </c>
       <c r="D95" s="89" t="s">
         <v>74</v>
       </c>
-      <c r="E95" s="156" t="s">
+      <c r="E95" s="155" t="s">
         <v>132</v>
       </c>
-      <c r="F95" s="199">
+      <c r="F95" s="138">
         <v>1.0</v>
       </c>
-      <c r="G95" s="200"/>
-      <c r="H95" s="140">
+      <c r="G95" s="92"/>
+      <c r="H95" s="139">
         <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="I95" s="200"/>
-      <c r="J95" s="163" t="s">
-        <v>67</v>
-      </c>
-      <c r="K95" s="186"/>
-      <c r="L95" s="186"/>
-      <c r="M95" s="201"/>
-      <c r="N95" s="202"/>
-      <c r="O95" s="202"/>
-      <c r="P95" s="201"/>
-      <c r="Q95" s="142">
+        <v>1.2</v>
+      </c>
+      <c r="I95" s="92"/>
+      <c r="J95" s="81" t="s">
+        <v>54</v>
+      </c>
+      <c r="K95" s="5"/>
+      <c r="L95" s="5"/>
+      <c r="M95" s="178">
+        <v>0.7</v>
+      </c>
+      <c r="N95" s="140">
+        <v>0.5</v>
+      </c>
+      <c r="O95" s="178" t="s">
+        <v>82</v>
+      </c>
+      <c r="P95" s="178" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q95" s="141">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="R95" s="5"/>
       <c r="S95" s="5"/>
@@ -6814,51 +6777,51 @@
       <c r="AF95" s="5"/>
     </row>
     <row r="96">
-      <c r="A96" s="215" t="s">
+      <c r="A96" s="180" t="s">
         <v>6</v>
       </c>
-      <c r="B96" s="215"/>
-      <c r="C96" s="216"/>
-      <c r="D96" s="216"/>
-      <c r="E96" s="217"/>
-      <c r="F96" s="218">
+      <c r="B96" s="180"/>
+      <c r="C96" s="181"/>
+      <c r="D96" s="181"/>
+      <c r="E96" s="182"/>
+      <c r="F96" s="183">
         <f t="shared" ref="F96:G96" si="21">SUM(F5:F95)</f>
         <v>235.5</v>
       </c>
-      <c r="G96" s="219">
+      <c r="G96" s="184">
         <f t="shared" si="21"/>
         <v>235.5</v>
       </c>
-      <c r="H96" s="220">
+      <c r="H96" s="185">
         <f t="shared" si="20"/>
-        <v>100.9</v>
-      </c>
-      <c r="I96" s="219">
+        <v>123.1</v>
+      </c>
+      <c r="I96" s="184">
         <f>SUM(I5:I95)</f>
-        <v>100.9</v>
-      </c>
-      <c r="J96" s="221"/>
-      <c r="K96" s="221"/>
-      <c r="L96" s="221"/>
-      <c r="M96" s="220">
+        <v>121.1</v>
+      </c>
+      <c r="J96" s="158"/>
+      <c r="K96" s="158"/>
+      <c r="L96" s="158"/>
+      <c r="M96" s="185">
         <f t="shared" ref="M96:P96" si="22">SUM(M5:M95)</f>
-        <v>37.15</v>
-      </c>
-      <c r="N96" s="220">
+        <v>54.35</v>
+      </c>
+      <c r="N96" s="185">
         <f t="shared" si="22"/>
-        <v>31.8</v>
-      </c>
-      <c r="O96" s="220">
+        <v>36.8</v>
+      </c>
+      <c r="O96" s="185">
         <f t="shared" si="22"/>
         <v>21.55</v>
       </c>
-      <c r="P96" s="220">
+      <c r="P96" s="185">
         <f t="shared" si="22"/>
         <v>10.4</v>
       </c>
-      <c r="Q96" s="220">
+      <c r="Q96" s="185">
         <f t="shared" si="17"/>
-        <v>100.9</v>
+        <v>123.1</v>
       </c>
       <c r="R96" s="5"/>
       <c r="S96" s="5"/>

</xml_diff>